<commit_message>
updated case study input files and tests for compatibility with the hydraulics module
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pareto\source_code\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA87C43E-DD5E-4A71-BA6C-4215E1F2CF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A83707-9A27-45A6-92DF-AC099A02156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="3480" windowWidth="28800" windowHeight="15195" tabRatio="834" firstSheet="27" activeTab="43" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="2820" yWindow="1935" windowWidth="28800" windowHeight="15195" tabRatio="834" firstSheet="23" activeTab="37" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="271">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -2223,20 +2223,8 @@
       <sheetData sheetId="36"/>
       <sheetData sheetId="37"/>
       <sheetData sheetId="38"/>
-      <sheetData sheetId="39">
-        <row r="3">
-          <cell r="B3">
-            <v>5000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="40">
-        <row r="3">
-          <cell r="N3">
-            <v>32000</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
       <sheetData sheetId="41"/>
       <sheetData sheetId="42"/>
       <sheetData sheetId="43"/>
@@ -5680,10 +5668,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B63"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5713,249 +5701,173 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="114"/>
-      <c r="B3" s="115"/>
+      <c r="A3" s="114" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="115">
+        <v>650</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="114"/>
-      <c r="B4" s="115"/>
+      <c r="A4" s="114" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="115">
+        <v>550</v>
+      </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="115"/>
+      <c r="A5" s="114" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="115">
+        <v>550</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="115"/>
+      <c r="A6" s="114" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="115">
+        <v>450</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="115"/>
+      <c r="A7" s="114" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="115">
+        <v>650</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="115"/>
+      <c r="A8" s="114" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="115">
+        <v>550</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="115"/>
+      <c r="A9" s="114" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="115">
+        <v>600</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="114"/>
-      <c r="B10" s="115"/>
+      <c r="A10" s="114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="115">
+        <v>650</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="114"/>
-      <c r="B11" s="115"/>
+      <c r="A11" s="114" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="115">
+        <v>650</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="114"/>
-      <c r="B12" s="115"/>
+      <c r="A12" s="114" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="115">
+        <v>350</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="114"/>
-      <c r="B13" s="115"/>
+      <c r="A13" s="114" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="115">
+        <v>500</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="114"/>
-      <c r="B14" s="115"/>
+      <c r="A14" s="114" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="115">
+        <v>250</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
-      <c r="B15" s="115"/>
+      <c r="A15" s="114" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="115">
+        <v>600</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="114"/>
-      <c r="B16" s="115"/>
+      <c r="A16" s="114" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="115">
+        <v>600</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="114"/>
-      <c r="B17" s="115"/>
+      <c r="A17" s="114" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="115">
+        <v>600</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="114"/>
-      <c r="B18" s="115"/>
+      <c r="A18" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="115">
+        <v>600</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="114"/>
-      <c r="B19" s="115"/>
+      <c r="A19" s="114" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="115">
+        <v>550</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="114"/>
-      <c r="B20" s="115"/>
+      <c r="A20" s="114" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="115">
+        <v>550</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="114"/>
-      <c r="B21" s="115"/>
+      <c r="A21" s="114" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="115">
+        <v>550</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="114"/>
-      <c r="B22" s="115"/>
+      <c r="A22" s="114" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="115">
+        <v>550</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="114"/>
-      <c r="B23" s="115"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="114"/>
-      <c r="B24" s="115"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="114"/>
-      <c r="B25" s="115"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="114"/>
-      <c r="B26" s="115"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="114"/>
-      <c r="B27" s="115"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="114"/>
-      <c r="B28" s="115"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="114"/>
-      <c r="B29" s="115"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="114"/>
-      <c r="B30" s="115"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="114"/>
-      <c r="B31" s="115"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="114"/>
-      <c r="B32" s="115"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="114"/>
-      <c r="B33" s="115"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="114"/>
-      <c r="B34" s="115"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="114"/>
-      <c r="B35" s="115"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="114"/>
-      <c r="B36" s="115"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="114"/>
-      <c r="B37" s="115"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="114"/>
-      <c r="B38" s="115"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="114"/>
-      <c r="B39" s="115"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="114"/>
-      <c r="B40" s="115"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="114"/>
-      <c r="B41" s="115"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="114"/>
-      <c r="B42" s="115"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="114"/>
-      <c r="B43" s="115"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="114"/>
-      <c r="B44" s="115"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="114"/>
-      <c r="B45" s="115"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="114"/>
-      <c r="B46" s="115"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="114"/>
-      <c r="B47" s="115"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="114"/>
-      <c r="B48" s="115"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="114"/>
-      <c r="B49" s="115"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="114"/>
-      <c r="B50" s="115"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="114"/>
-      <c r="B51" s="115"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="114"/>
-      <c r="B52" s="115"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="114"/>
-      <c r="B53" s="115"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="114"/>
-      <c r="B54" s="115"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="114"/>
-      <c r="B55" s="115"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="114"/>
-      <c r="B56" s="115"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="114"/>
-      <c r="B57" s="115"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="114"/>
-      <c r="B58" s="115"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="114"/>
-      <c r="B59" s="115"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="114"/>
-      <c r="B60" s="115"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="114"/>
-      <c r="B61" s="115"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="114"/>
-      <c r="B62" s="115"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="114"/>
-      <c r="B63" s="115"/>
+      <c r="A23" s="114" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="115">
+        <v>500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6419,7 +6331,9 @@
   </sheetPr>
   <dimension ref="A1:BA10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:BA2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7474,7 +7388,7 @@
   <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7853,7 +7767,7 @@
   <dimension ref="A1:BC23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:BA2"/>
+      <selection activeCell="B3" sqref="B3:BA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7887,340 +7801,1234 @@
       <c r="A2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5"/>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="25"/>
+      <c r="B2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="AO2" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP2" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="BA2" s="25" t="s">
+        <v>232</v>
+      </c>
       <c r="BC2" s="1"/>
     </row>
     <row r="3" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="34"/>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="34"/>
-      <c r="AE3" s="34"/>
-      <c r="AF3" s="34"/>
-      <c r="AG3" s="34"/>
-      <c r="AH3" s="34"/>
-      <c r="AI3" s="34"/>
-      <c r="AJ3" s="34"/>
-      <c r="AK3" s="34"/>
-      <c r="AL3" s="34"/>
-      <c r="AM3" s="34"/>
-      <c r="AN3" s="34"/>
-      <c r="AO3" s="34"/>
-      <c r="AP3" s="34"/>
-      <c r="AQ3" s="34"/>
-      <c r="AR3" s="34"/>
-      <c r="AS3" s="34"/>
-      <c r="AT3" s="34"/>
-      <c r="AU3" s="34"/>
-      <c r="AV3" s="34"/>
-      <c r="AW3" s="34"/>
-      <c r="AX3" s="34"/>
-      <c r="AY3" s="34"/>
-      <c r="AZ3" s="34"/>
-      <c r="BA3" s="35"/>
+      <c r="A3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="34">
+        <f>PadRates!B3*WellPressure!$Q$1</f>
+        <v>50</v>
+      </c>
+      <c r="C3" s="34">
+        <f>PadRates!C3*WellPressure!$Q$1</f>
+        <v>43.226861565393257</v>
+      </c>
+      <c r="D3" s="34">
+        <f>PadRates!D3*WellPressure!$Q$1</f>
+        <v>39.698540540280661</v>
+      </c>
+      <c r="E3" s="34">
+        <f>PadRates!E3*WellPressure!$Q$1</f>
+        <v>37.371231215873465</v>
+      </c>
+      <c r="F3" s="34">
+        <f>PadRates!F3*WellPressure!$Q$1</f>
+        <v>35.660407645411759</v>
+      </c>
+      <c r="G3" s="34">
+        <f>PadRates!G3*WellPressure!$Q$1</f>
+        <v>34.320866325657292</v>
+      </c>
+      <c r="H3" s="34">
+        <f>PadRates!H3*WellPressure!$Q$1</f>
+        <v>33.227633834431956</v>
+      </c>
+      <c r="I3" s="34">
+        <f>PadRates!I3*WellPressure!$Q$1</f>
+        <v>32.308820765937305</v>
+      </c>
+      <c r="J3" s="34">
+        <f>PadRates!J3*WellPressure!$Q$1</f>
+        <v>31.519482420566142</v>
+      </c>
+      <c r="K3" s="34">
+        <f>PadRates!K3*WellPressure!$Q$1</f>
+        <v>30.829750093074107</v>
+      </c>
+      <c r="L3" s="34">
+        <f>PadRates!L3*WellPressure!$Q$1</f>
+        <v>30.218822690895305</v>
+      </c>
+      <c r="M3" s="34">
+        <f>PadRates!M3*WellPressure!$Q$1</f>
+        <v>29.6716667492711</v>
+      </c>
+      <c r="N3" s="34">
+        <f>PadRates!N3*WellPressure!$Q$1</f>
+        <v>29.177084983850378</v>
+      </c>
+      <c r="O3" s="34">
+        <f>PadRates!O3*WellPressure!$Q$1</f>
+        <v>28.726526558131351</v>
+      </c>
+      <c r="P3" s="34">
+        <f>PadRates!P3*WellPressure!$Q$1</f>
+        <v>28.313322771886266</v>
+      </c>
+      <c r="Q3" s="34">
+        <f>PadRates!Q3*WellPressure!$Q$1</f>
+        <v>27.932178451805498</v>
+      </c>
+      <c r="R3" s="34">
+        <f>PadRates!R3*WellPressure!$Q$1</f>
+        <v>27.578823208879022</v>
+      </c>
+      <c r="S3" s="34">
+        <f>PadRates!S3*WellPressure!$Q$1</f>
+        <v>27.249766064133187</v>
+      </c>
+      <c r="T3" s="34">
+        <f>PadRates!T3*WellPressure!$Q$1</f>
+        <v>26.942118882559804</v>
+      </c>
+      <c r="U3" s="34">
+        <f>PadRates!U3*WellPressure!$Q$1</f>
+        <v>26.653466787379696</v>
+      </c>
+      <c r="V3" s="34">
+        <f>PadRates!V3*WellPressure!$Q$1</f>
+        <v>26.381771376675967</v>
+      </c>
+      <c r="W3" s="34">
+        <f>PadRates!W3*WellPressure!$Q$1</f>
+        <v>26.125297302569919</v>
+      </c>
+      <c r="X3" s="34">
+        <f>PadRates!X3*WellPressure!$Q$1</f>
+        <v>25.882555787844932</v>
+      </c>
+      <c r="Y3" s="34">
+        <f>PadRates!Y3*WellPressure!$Q$1</f>
+        <v>25.652260619704474</v>
+      </c>
+      <c r="Z3" s="34">
+        <f>PadRates!Z3*WellPressure!$Q$1</f>
+        <v>25.433293468738825</v>
+      </c>
+      <c r="AA3" s="34">
+        <f>PadRates!AA3*WellPressure!$Q$1</f>
+        <v>25.224676269572292</v>
+      </c>
+      <c r="AB3" s="34">
+        <f>PadRates!AB3*WellPressure!$Q$1</f>
+        <v>25.025549013630176</v>
+      </c>
+      <c r="AC3" s="34">
+        <f>PadRates!AC3*WellPressure!$Q$1</f>
+        <v>24.83515173565873</v>
+      </c>
+      <c r="AD3" s="34">
+        <f>PadRates!AD3*WellPressure!$Q$1</f>
+        <v>24.652809782959771</v>
+      </c>
+      <c r="AE3" s="34">
+        <f>PadRates!AE3*WellPressure!$Q$1</f>
+        <v>24.477921678332478</v>
+      </c>
+      <c r="AF3" s="34">
+        <f>PadRates!AF3*WellPressure!$Q$1</f>
+        <v>24.309949050140045</v>
+      </c>
+      <c r="AG3" s="34">
+        <f>PadRates!AG3*WellPressure!$Q$1</f>
+        <v>24.148408223121137</v>
+      </c>
+      <c r="AH3" s="34">
+        <f>PadRates!AH3*WellPressure!$Q$1</f>
+        <v>23.99286315348121</v>
+      </c>
+      <c r="AI3" s="34">
+        <f>PadRates!AI3*WellPressure!$Q$1</f>
+        <v>23.842919459733363</v>
+      </c>
+      <c r="AJ3" s="34">
+        <f>PadRates!AJ3*WellPressure!$Q$1</f>
+        <v>23.69821935256639</v>
+      </c>
+      <c r="AK3" s="34">
+        <f>PadRates!AK3*WellPressure!$Q$1</f>
+        <v>23.55843730687273</v>
+      </c>
+      <c r="AL3" s="34">
+        <f>PadRates!AL3*WellPressure!$Q$1</f>
+        <v>23.423276349980757</v>
+      </c>
+      <c r="AM3" s="34">
+        <f>PadRates!AM3*WellPressure!$Q$1</f>
+        <v>23.292464864295606</v>
+      </c>
+      <c r="AN3" s="34">
+        <f>PadRates!AN3*WellPressure!$Q$1</f>
+        <v>23.165753821571975</v>
+      </c>
+      <c r="AO3" s="34">
+        <f>PadRates!AO3*WellPressure!$Q$1</f>
+        <v>23.042914381117377</v>
+      </c>
+      <c r="AP3" s="34">
+        <f>PadRates!AP3*WellPressure!$Q$1</f>
+        <v>22.923735796250238</v>
+      </c>
+      <c r="AQ3" s="34">
+        <f>PadRates!AQ3*WellPressure!$Q$1</f>
+        <v>22.808023582988522</v>
+      </c>
+      <c r="AR3" s="34">
+        <f>PadRates!AR3*WellPressure!$Q$1</f>
+        <v>22.695597912736286</v>
+      </c>
+      <c r="AS3" s="34">
+        <f>PadRates!AS3*WellPressure!$Q$1</f>
+        <v>22.586292197058636</v>
+      </c>
+      <c r="AT3" s="34">
+        <f>PadRates!AT3*WellPressure!$Q$1</f>
+        <v>22.479951837795571</v>
+      </c>
+      <c r="AU3" s="34">
+        <f>PadRates!AU3*WellPressure!$Q$1</f>
+        <v>22.376433119994818</v>
+      </c>
+      <c r="AV3" s="34">
+        <f>PadRates!AV3*WellPressure!$Q$1</f>
+        <v>22.275602228629186</v>
+      </c>
+      <c r="AW3" s="34">
+        <f>PadRates!AW3*WellPressure!$Q$1</f>
+        <v>22.177334372947094</v>
+      </c>
+      <c r="AX3" s="34">
+        <f>PadRates!AX3*WellPressure!$Q$1</f>
+        <v>22.081513004701744</v>
+      </c>
+      <c r="AY3" s="34">
+        <f>PadRates!AY3*WellPressure!$Q$1</f>
+        <v>21.988029118503878</v>
+      </c>
+      <c r="AZ3" s="34">
+        <f>PadRates!AZ3*WellPressure!$Q$1</f>
+        <v>21.896780624218341</v>
+      </c>
+      <c r="BA3" s="34">
+        <f>PadRates!BA3*WellPressure!$Q$1</f>
+        <v>21.807671782733241</v>
+      </c>
       <c r="BB3" s="84"/>
       <c r="BC3" s="1"/>
     </row>
     <row r="4" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="34"/>
-      <c r="AS4" s="34"/>
-      <c r="AT4" s="34"/>
-      <c r="AU4" s="34"/>
-      <c r="AV4" s="34"/>
-      <c r="AW4" s="34"/>
-      <c r="AX4" s="34"/>
-      <c r="AY4" s="34"/>
-      <c r="AZ4" s="34"/>
-      <c r="BA4" s="35"/>
+      <c r="A4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="34">
+        <f>PadRates!B4*WellPressure!$Q$1</f>
+        <v>130</v>
+      </c>
+      <c r="C4" s="34">
+        <f>PadRates!C4*WellPressure!$Q$1</f>
+        <v>101.99593272657759</v>
+      </c>
+      <c r="D4" s="34">
+        <f>PadRates!D4*WellPressure!$Q$1</f>
+        <v>88.501557384298565</v>
+      </c>
+      <c r="E4" s="34">
+        <f>PadRates!E4*WellPressure!$Q$1</f>
+        <v>80.024386867419565</v>
+      </c>
+      <c r="F4" s="34">
+        <f>PadRates!F4*WellPressure!$Q$1</f>
+        <v>74.012291525269902</v>
+      </c>
+      <c r="G4" s="34">
+        <f>PadRates!G4*WellPressure!$Q$1</f>
+        <v>69.436914562817392</v>
+      </c>
+      <c r="H4" s="34">
+        <f>PadRates!H4*WellPressure!$Q$1</f>
+        <v>65.789871524644781</v>
+      </c>
+      <c r="I4" s="34">
+        <f>PadRates!I4*WellPressure!$Q$1</f>
+        <v>62.785861380114973</v>
+      </c>
+      <c r="J4" s="34">
+        <f>PadRates!J4*WellPressure!$Q$1</f>
+        <v>60.25019738035607</v>
+      </c>
+      <c r="K4" s="34">
+        <f>PadRates!K4*WellPressure!$Q$1</f>
+        <v>58.068866979625213</v>
+      </c>
+      <c r="L4" s="34">
+        <f>PadRates!L4*WellPressure!$Q$1</f>
+        <v>56.163726073325101</v>
+      </c>
+      <c r="M4" s="34">
+        <f>PadRates!M4*WellPressure!$Q$1</f>
+        <v>54.47909897300184</v>
+      </c>
+      <c r="N4" s="34">
+        <f>PadRates!N4*WellPressure!$Q$1</f>
+        <v>52.974050229787558</v>
+      </c>
+      <c r="O4" s="34">
+        <f>PadRates!O4*WellPressure!$Q$1</f>
+        <v>51.617687000906557</v>
+      </c>
+      <c r="P4" s="34">
+        <f>PadRates!P4*WellPressure!$Q$1</f>
+        <v>50.386177427439279</v>
+      </c>
+      <c r="Q4" s="34">
+        <f>PadRates!Q4*WellPressure!$Q$1</f>
+        <v>49.260788411587946</v>
+      </c>
+      <c r="R4" s="34">
+        <f>PadRates!R4*WellPressure!$Q$1</f>
+        <v>48.226553894531484</v>
+      </c>
+      <c r="S4" s="34">
+        <f>PadRates!S4*WellPressure!$Q$1</f>
+        <v>47.271346759767852</v>
+      </c>
+      <c r="T4" s="34">
+        <f>PadRates!T4*WellPressure!$Q$1</f>
+        <v>46.385216926550754</v>
+      </c>
+      <c r="U4" s="34">
+        <f>PadRates!U4*WellPressure!$Q$1</f>
+        <v>45.55990961509567</v>
+      </c>
+      <c r="V4" s="34">
+        <f>PadRates!V4*WellPressure!$Q$1</f>
+        <v>44.788508384953687</v>
+      </c>
+      <c r="W4" s="34">
+        <f>PadRates!W4*WellPressure!$Q$1</f>
+        <v>44.065166355759992</v>
+      </c>
+      <c r="X4" s="34">
+        <f>PadRates!X4*WellPressure!$Q$1</f>
+        <v>43.38490089293451</v>
+      </c>
+      <c r="Y4" s="34">
+        <f>PadRates!Y4*WellPressure!$Q$1</f>
+        <v>42.743434721960448</v>
+      </c>
+      <c r="Z4" s="34">
+        <f>PadRates!Z4*WellPressure!$Q$1</f>
+        <v>42.137071514011829</v>
+      </c>
+      <c r="AA4" s="34">
+        <f>PadRates!AA4*WellPressure!$Q$1</f>
+        <v>41.562597411475018</v>
+      </c>
+      <c r="AB4" s="34">
+        <f>PadRates!AB4*WellPressure!$Q$1</f>
+        <v>41.017202314406909</v>
+      </c>
+      <c r="AC4" s="34">
+        <f>PadRates!AC4*WellPressure!$Q$1</f>
+        <v>40.498416391123101</v>
+      </c>
+      <c r="AD4" s="34">
+        <f>PadRates!AD4*WellPressure!$Q$1</f>
+        <v>40.004058439727949</v>
+      </c>
+      <c r="AE4" s="34">
+        <f>PadRates!AE4*WellPressure!$Q$1</f>
+        <v>39.532193563373077</v>
+      </c>
+      <c r="AF4" s="34">
+        <f>PadRates!AF4*WellPressure!$Q$1</f>
+        <v>39.081098230304683</v>
+      </c>
+      <c r="AG4" s="34">
+        <f>PadRates!AG4*WellPressure!$Q$1</f>
+        <v>38.649231237588431</v>
+      </c>
+      <c r="AH4" s="34">
+        <f>PadRates!AH4*WellPressure!$Q$1</f>
+        <v>38.235209430726201</v>
+      </c>
+      <c r="AI4" s="34">
+        <f>PadRates!AI4*WellPressure!$Q$1</f>
+        <v>37.837787282010005</v>
+      </c>
+      <c r="AJ4" s="34">
+        <f>PadRates!AJ4*WellPressure!$Q$1</f>
+        <v>37.455839620708169</v>
+      </c>
+      <c r="AK4" s="34">
+        <f>PadRates!AK4*WellPressure!$Q$1</f>
+        <v>37.08834695387695</v>
+      </c>
+      <c r="AL4" s="34">
+        <f>PadRates!AL4*WellPressure!$Q$1</f>
+        <v>36.73438292910491</v>
+      </c>
+      <c r="AM4" s="34">
+        <f>PadRates!AM4*WellPressure!$Q$1</f>
+        <v>36.393103578062913</v>
+      </c>
+      <c r="AN4" s="34">
+        <f>PadRates!AN4*WellPressure!$Q$1</f>
+        <v>36.063738048386597</v>
+      </c>
+      <c r="AO4" s="34">
+        <f>PadRates!AO4*WellPressure!$Q$1</f>
+        <v>35.74558058561734</v>
+      </c>
+      <c r="AP4" s="34">
+        <f>PadRates!AP4*WellPressure!$Q$1</f>
+        <v>35.437983569997165</v>
+      </c>
+      <c r="AQ4" s="34">
+        <f>PadRates!AQ4*WellPressure!$Q$1</f>
+        <v>35.140351447349943</v>
+      </c>
+      <c r="AR4" s="34">
+        <f>PadRates!AR4*WellPressure!$Q$1</f>
+        <v>34.852135420978044</v>
+      </c>
+      <c r="AS4" s="34">
+        <f>PadRates!AS4*WellPressure!$Q$1</f>
+        <v>34.5728287939042</v>
+      </c>
+      <c r="AT4" s="34">
+        <f>PadRates!AT4*WellPressure!$Q$1</f>
+        <v>34.301962868999745</v>
+      </c>
+      <c r="AU4" s="34">
+        <f>PadRates!AU4*WellPressure!$Q$1</f>
+        <v>34.039103329422957</v>
+      </c>
+      <c r="AV4" s="34">
+        <f>PadRates!AV4*WellPressure!$Q$1</f>
+        <v>33.783847034009874</v>
+      </c>
+      <c r="AW4" s="34">
+        <f>PadRates!AW4*WellPressure!$Q$1</f>
+        <v>33.535819172337995</v>
+      </c>
+      <c r="AX4" s="34">
+        <f>PadRates!AX4*WellPressure!$Q$1</f>
+        <v>33.294670732532815</v>
+      </c>
+      <c r="AY4" s="34">
+        <f>PadRates!AY4*WellPressure!$Q$1</f>
+        <v>33.060076241831837</v>
+      </c>
+      <c r="AZ4" s="34">
+        <f>PadRates!AZ4*WellPressure!$Q$1</f>
+        <v>32.831731745721875</v>
+      </c>
+      <c r="BA4" s="34">
+        <f>PadRates!BA4*WellPressure!$Q$1</f>
+        <v>32.609352996327956</v>
+      </c>
       <c r="BB4" s="84"/>
       <c r="BC4" s="1"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="34"/>
-      <c r="W5" s="34"/>
-      <c r="X5" s="34"/>
-      <c r="Y5" s="34"/>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="34"/>
-      <c r="AE5" s="34"/>
-      <c r="AF5" s="34"/>
-      <c r="AG5" s="34"/>
-      <c r="AH5" s="34"/>
-      <c r="AI5" s="34"/>
-      <c r="AJ5" s="34"/>
-      <c r="AK5" s="34"/>
-      <c r="AL5" s="34"/>
-      <c r="AM5" s="34"/>
-      <c r="AN5" s="34"/>
-      <c r="AO5" s="34"/>
-      <c r="AP5" s="34"/>
-      <c r="AQ5" s="34"/>
-      <c r="AR5" s="34"/>
-      <c r="AS5" s="34"/>
-      <c r="AT5" s="34"/>
-      <c r="AU5" s="34"/>
-      <c r="AV5" s="34"/>
-      <c r="AW5" s="34"/>
-      <c r="AX5" s="34"/>
-      <c r="AY5" s="34"/>
-      <c r="AZ5" s="34"/>
-      <c r="BA5" s="35"/>
+      <c r="A5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="34">
+        <f>PadRates!B5*WellPressure!$Q$1</f>
+        <v>80</v>
+      </c>
+      <c r="C5" s="34">
+        <f>PadRates!C5*WellPressure!$Q$1</f>
+        <v>67.271713220297173</v>
+      </c>
+      <c r="D5" s="34">
+        <f>PadRates!D5*WellPressure!$Q$1</f>
+        <v>60.786854852127398</v>
+      </c>
+      <c r="E5" s="34">
+        <f>PadRates!E5*WellPressure!$Q$1</f>
+        <v>56.568542494923804</v>
+      </c>
+      <c r="F5" s="34">
+        <f>PadRates!F5*WellPressure!$Q$1</f>
+        <v>53.499224398113761</v>
+      </c>
+      <c r="G5" s="34">
+        <f>PadRates!G5*WellPressure!$Q$1</f>
+        <v>51.1154483397018</v>
+      </c>
+      <c r="H5" s="34">
+        <f>PadRates!H5*WellPressure!$Q$1</f>
+        <v>49.183052236101162</v>
+      </c>
+      <c r="I5" s="34">
+        <f>PadRates!I5*WellPressure!$Q$1</f>
+        <v>47.568284600108846</v>
+      </c>
+      <c r="J5" s="34">
+        <f>PadRates!J5*WellPressure!$Q$1</f>
+        <v>46.188021535170058</v>
+      </c>
+      <c r="K5" s="34">
+        <f>PadRates!K5*WellPressure!$Q$1</f>
+        <v>44.987306015227922</v>
+      </c>
+      <c r="L5" s="34">
+        <f>PadRates!L5*WellPressure!$Q$1</f>
+        <v>43.928038942088996</v>
+      </c>
+      <c r="M5" s="34">
+        <f>PadRates!M5*WellPressure!$Q$1</f>
+        <v>42.982797272941681</v>
+      </c>
+      <c r="N5" s="34">
+        <f>PadRates!N5*WellPressure!$Q$1</f>
+        <v>42.131231027834126</v>
+      </c>
+      <c r="O5" s="34">
+        <f>PadRates!O5*WellPressure!$Q$1</f>
+        <v>41.357852316573648</v>
+      </c>
+      <c r="P5" s="34">
+        <f>PadRates!P5*WellPressure!$Q$1</f>
+        <v>40.650619852369175</v>
+      </c>
+      <c r="Q5" s="34">
+        <f>PadRates!Q5*WellPressure!$Q$1</f>
+        <v>40</v>
+      </c>
+      <c r="R5" s="34">
+        <f>PadRates!R5*WellPressure!$Q$1</f>
+        <v>39.398324840436189</v>
+      </c>
+      <c r="S5" s="34">
+        <f>PadRates!S5*WellPressure!$Q$1</f>
+        <v>38.839341736585872</v>
+      </c>
+      <c r="T5" s="34">
+        <f>PadRates!T5*WellPressure!$Q$1</f>
+        <v>38.317890035485973</v>
+      </c>
+      <c r="U5" s="34">
+        <f>PadRates!U5*WellPressure!$Q$1</f>
+        <v>37.829664360127033</v>
+      </c>
+      <c r="V5" s="34">
+        <f>PadRates!V5*WellPressure!$Q$1</f>
+        <v>37.371038218256011</v>
+      </c>
+      <c r="W5" s="34">
+        <f>PadRates!W5*WellPressure!$Q$1</f>
+        <v>36.93893047552821</v>
+      </c>
+      <c r="X5" s="34">
+        <f>PadRates!X5*WellPressure!$Q$1</f>
+        <v>36.530702839738503</v>
+      </c>
+      <c r="Y5" s="34">
+        <f>PadRates!Y5*WellPressure!$Q$1</f>
+        <v>36.14408014439379</v>
+      </c>
+      <c r="Z5" s="34">
+        <f>PadRates!Z5*WellPressure!$Q$1</f>
+        <v>35.777087639996637</v>
+      </c>
+      <c r="AA5" s="34">
+        <f>PadRates!AA5*WellPressure!$Q$1</f>
+        <v>35.428001141531794</v>
+      </c>
+      <c r="AB5" s="34">
+        <f>PadRates!AB5*WellPressure!$Q$1</f>
+        <v>35.095307012066471</v>
+      </c>
+      <c r="AC5" s="34">
+        <f>PadRates!AC5*WellPressure!$Q$1</f>
+        <v>34.777669755599312</v>
+      </c>
+      <c r="AD5" s="34">
+        <f>PadRates!AD5*WellPressure!$Q$1</f>
+        <v>34.473905556712481</v>
+      </c>
+      <c r="AE5" s="34">
+        <f>PadRates!AE5*WellPressure!$Q$1</f>
+        <v>34.182960511698724</v>
+      </c>
+      <c r="AF5" s="34">
+        <f>PadRates!AF5*WellPressure!$Q$1</f>
+        <v>33.903892593201732</v>
+      </c>
+      <c r="AG5" s="34">
+        <f>PadRates!AG5*WellPressure!$Q$1</f>
+        <v>33.635856610148586</v>
+      </c>
+      <c r="AH5" s="34">
+        <f>PadRates!AH5*WellPressure!$Q$1</f>
+        <v>33.378091588892048</v>
+      </c>
+      <c r="AI5" s="34">
+        <f>PadRates!AI5*WellPressure!$Q$1</f>
+        <v>33.129910125324166</v>
+      </c>
+      <c r="AJ5" s="34">
+        <f>PadRates!AJ5*WellPressure!$Q$1</f>
+        <v>32.890689352041584</v>
+      </c>
+      <c r="AK5" s="34">
+        <f>PadRates!AK5*WellPressure!$Q$1</f>
+        <v>32.65986323710905</v>
+      </c>
+      <c r="AL5" s="34">
+        <f>PadRates!AL5*WellPressure!$Q$1</f>
+        <v>32.436915987101592</v>
+      </c>
+      <c r="AM5" s="34">
+        <f>PadRates!AM5*WellPressure!$Q$1</f>
+        <v>32.221376370926187</v>
+      </c>
+      <c r="AN5" s="34">
+        <f>PadRates!AN5*WellPressure!$Q$1</f>
+        <v>32.012812815379995</v>
+      </c>
+      <c r="AO5" s="34">
+        <f>PadRates!AO5*WellPressure!$Q$1</f>
+        <v>31.810829150682025</v>
+      </c>
+      <c r="AP5" s="34">
+        <f>PadRates!AP5*WellPressure!$Q$1</f>
+        <v>31.615060905952383</v>
+      </c>
+      <c r="AQ5" s="34">
+        <f>PadRates!AQ5*WellPressure!$Q$1</f>
+        <v>31.425172072041036</v>
+      </c>
+      <c r="AR5" s="34">
+        <f>PadRates!AR5*WellPressure!$Q$1</f>
+        <v>31.24085226316129</v>
+      </c>
+      <c r="AS5" s="34">
+        <f>PadRates!AS5*WellPressure!$Q$1</f>
+        <v>31.061814220177858</v>
+      </c>
+      <c r="AT5" s="34">
+        <f>PadRates!AT5*WellPressure!$Q$1</f>
+        <v>30.887791607687177</v>
+      </c>
+      <c r="AU5" s="34">
+        <f>PadRates!AU5*WellPressure!$Q$1</f>
+        <v>30.718537064634798</v>
+      </c>
+      <c r="AV5" s="34">
+        <f>PadRates!AV5*WellPressure!$Q$1</f>
+        <v>30.553820474476272</v>
+      </c>
+      <c r="AW5" s="34">
+        <f>PadRates!AW5*WellPressure!$Q$1</f>
+        <v>30.393427426063699</v>
+      </c>
+      <c r="AX5" s="34">
+        <f>PadRates!AX5*WellPressure!$Q$1</f>
+        <v>30.237157840738181</v>
+      </c>
+      <c r="AY5" s="34">
+        <f>PadRates!AY5*WellPressure!$Q$1</f>
+        <v>30.084824744691151</v>
+      </c>
+      <c r="AZ5" s="34">
+        <f>PadRates!AZ5*WellPressure!$Q$1</f>
+        <v>29.936253168657</v>
+      </c>
+      <c r="BA5" s="34">
+        <f>PadRates!BA5*WellPressure!$Q$1</f>
+        <v>29.791279159518584</v>
+      </c>
       <c r="BB5" s="84"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="34"/>
-      <c r="AC6" s="34"/>
-      <c r="AD6" s="34"/>
-      <c r="AE6" s="34"/>
-      <c r="AF6" s="34"/>
-      <c r="AG6" s="34"/>
-      <c r="AH6" s="34"/>
-      <c r="AI6" s="34"/>
-      <c r="AJ6" s="34"/>
-      <c r="AK6" s="34"/>
-      <c r="AL6" s="34"/>
-      <c r="AM6" s="34"/>
-      <c r="AN6" s="34"/>
-      <c r="AO6" s="34"/>
-      <c r="AP6" s="34"/>
-      <c r="AQ6" s="34"/>
-      <c r="AR6" s="34"/>
-      <c r="AS6" s="34"/>
-      <c r="AT6" s="34"/>
-      <c r="AU6" s="34"/>
-      <c r="AV6" s="34"/>
-      <c r="AW6" s="34"/>
-      <c r="AX6" s="34"/>
-      <c r="AY6" s="34"/>
-      <c r="AZ6" s="34"/>
-      <c r="BA6" s="35"/>
+      <c r="A6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="34">
+        <f>PadRates!B6*WellPressure!$Q$1</f>
+        <v>20</v>
+      </c>
+      <c r="C6" s="34">
+        <f>PadRates!C6*WellPressure!$Q$1</f>
+        <v>19.724654089867183</v>
+      </c>
+      <c r="D6" s="34">
+        <f>PadRates!D6*WellPressure!$Q$1</f>
+        <v>19.565347714583421</v>
+      </c>
+      <c r="E6" s="34">
+        <f>PadRates!E6*WellPressure!$Q$1</f>
+        <v>19.45309894824571</v>
+      </c>
+      <c r="F6" s="34">
+        <f>PadRates!F6*WellPressure!$Q$1</f>
+        <v>19.366475714512596</v>
+      </c>
+      <c r="G6" s="34">
+        <f>PadRates!G6*WellPressure!$Q$1</f>
+        <v>19.29598579090657</v>
+      </c>
+      <c r="H6" s="34">
+        <f>PadRates!H6*WellPressure!$Q$1</f>
+        <v>19.236587614095988</v>
+      </c>
+      <c r="I6" s="34">
+        <f>PadRates!I6*WellPressure!$Q$1</f>
+        <v>19.185282386505289</v>
+      </c>
+      <c r="J6" s="34">
+        <f>PadRates!J6*WellPressure!$Q$1</f>
+        <v>19.14014155962774</v>
+      </c>
+      <c r="K6" s="34">
+        <f>PadRates!K6*WellPressure!$Q$1</f>
+        <v>19.099851720428717</v>
+      </c>
+      <c r="L6" s="34">
+        <f>PadRates!L6*WellPressure!$Q$1</f>
+        <v>19.063478193082773</v>
+      </c>
+      <c r="M6" s="34">
+        <f>PadRates!M6*WellPressure!$Q$1</f>
+        <v>19.030332252431219</v>
+      </c>
+      <c r="N6" s="34">
+        <f>PadRates!N6*WellPressure!$Q$1</f>
+        <v>18.999891837835946</v>
+      </c>
+      <c r="O6" s="34">
+        <f>PadRates!O6*WellPressure!$Q$1</f>
+        <v>18.971751827873344</v>
+      </c>
+      <c r="P6" s="34">
+        <f>PadRates!P6*WellPressure!$Q$1</f>
+        <v>18.945591568023726</v>
+      </c>
+      <c r="Q6" s="34">
+        <f>PadRates!Q6*WellPressure!$Q$1</f>
+        <v>18.92115293451192</v>
+      </c>
+      <c r="R6" s="34">
+        <f>PadRates!R6*WellPressure!$Q$1</f>
+        <v>18.898225082424748</v>
+      </c>
+      <c r="S6" s="34">
+        <f>PadRates!S6*WellPressure!$Q$1</f>
+        <v>18.876633574737408</v>
+      </c>
+      <c r="T6" s="34">
+        <f>PadRates!T6*WellPressure!$Q$1</f>
+        <v>18.856232464552253</v>
+      </c>
+      <c r="U6" s="34">
+        <f>PadRates!U6*WellPressure!$Q$1</f>
+        <v>18.836898417660557</v>
+      </c>
+      <c r="V6" s="34">
+        <f>PadRates!V6*WellPressure!$Q$1</f>
+        <v>18.818526275591836</v>
+      </c>
+      <c r="W6" s="34">
+        <f>PadRates!W6*WellPressure!$Q$1</f>
+        <v>18.8010256554142</v>
+      </c>
+      <c r="X6" s="34">
+        <f>PadRates!X6*WellPressure!$Q$1</f>
+        <v>18.784318308654296</v>
+      </c>
+      <c r="Y6" s="34">
+        <f>PadRates!Y6*WellPressure!$Q$1</f>
+        <v>18.768336044722442</v>
+      </c>
+      <c r="Z6" s="34">
+        <f>PadRates!Z6*WellPressure!$Q$1</f>
+        <v>18.75301908004031</v>
+      </c>
+      <c r="AA6" s="34">
+        <f>PadRates!AA6*WellPressure!$Q$1</f>
+        <v>18.738314712310245</v>
+      </c>
+      <c r="AB6" s="34">
+        <f>PadRates!AB6*WellPressure!$Q$1</f>
+        <v>18.724176246023287</v>
+      </c>
+      <c r="AC6" s="34">
+        <f>PadRates!AC6*WellPressure!$Q$1</f>
+        <v>18.710562114180359</v>
+      </c>
+      <c r="AD6" s="34">
+        <f>PadRates!AD6*WellPressure!$Q$1</f>
+        <v>18.697435154762537</v>
+      </c>
+      <c r="AE6" s="34">
+        <f>PadRates!AE6*WellPressure!$Q$1</f>
+        <v>18.684762010358615</v>
+      </c>
+      <c r="AF6" s="34">
+        <f>PadRates!AF6*WellPressure!$Q$1</f>
+        <v>18.672512626632653</v>
+      </c>
+      <c r="AG6" s="34">
+        <f>PadRates!AG6*WellPressure!$Q$1</f>
+        <v>18.660659830736151</v>
+      </c>
+      <c r="AH6" s="34">
+        <f>PadRates!AH6*WellPressure!$Q$1</f>
+        <v>18.649178974852152</v>
+      </c>
+      <c r="AI6" s="34">
+        <f>PadRates!AI6*WellPressure!$Q$1</f>
+        <v>18.638047633163993</v>
+      </c>
+      <c r="AJ6" s="34">
+        <f>PadRates!AJ6*WellPressure!$Q$1</f>
+        <v>18.627245342924191</v>
+      </c>
+      <c r="AK6" s="34">
+        <f>PadRates!AK6*WellPressure!$Q$1</f>
+        <v>18.616753382143422</v>
+      </c>
+      <c r="AL6" s="34">
+        <f>PadRates!AL6*WellPressure!$Q$1</f>
+        <v>18.606554577858702</v>
+      </c>
+      <c r="AM6" s="34">
+        <f>PadRates!AM6*WellPressure!$Q$1</f>
+        <v>18.59663314007085</v>
+      </c>
+      <c r="AN6" s="34">
+        <f>PadRates!AN6*WellPressure!$Q$1</f>
+        <v>18.586974517336788</v>
+      </c>
+      <c r="AO6" s="34">
+        <f>PadRates!AO6*WellPressure!$Q$1</f>
+        <v>18.577565270716047</v>
+      </c>
+      <c r="AP6" s="34">
+        <f>PadRates!AP6*WellPressure!$Q$1</f>
+        <v>18.568392963342752</v>
+      </c>
+      <c r="AQ6" s="34">
+        <f>PadRates!AQ6*WellPressure!$Q$1</f>
+        <v>18.559446063356276</v>
+      </c>
+      <c r="AR6" s="34">
+        <f>PadRates!AR6*WellPressure!$Q$1</f>
+        <v>18.550713858298163</v>
+      </c>
+      <c r="AS6" s="34">
+        <f>PadRates!AS6*WellPressure!$Q$1</f>
+        <v>18.54218637938818</v>
+      </c>
+      <c r="AT6" s="34">
+        <f>PadRates!AT6*WellPressure!$Q$1</f>
+        <v>18.533854334343193</v>
+      </c>
+      <c r="AU6" s="34">
+        <f>PadRates!AU6*WellPressure!$Q$1</f>
+        <v>18.525709047608249</v>
+      </c>
+      <c r="AV6" s="34">
+        <f>PadRates!AV6*WellPressure!$Q$1</f>
+        <v>18.517742407040306</v>
+      </c>
+      <c r="AW6" s="34">
+        <f>PadRates!AW6*WellPressure!$Q$1</f>
+        <v>18.509946816226808</v>
+      </c>
+      <c r="AX6" s="34">
+        <f>PadRates!AX6*WellPressure!$Q$1</f>
+        <v>18.502315151739563</v>
+      </c>
+      <c r="AY6" s="34">
+        <f>PadRates!AY6*WellPressure!$Q$1</f>
+        <v>18.494840724723719</v>
+      </c>
+      <c r="AZ6" s="34">
+        <f>PadRates!AZ6*WellPressure!$Q$1</f>
+        <v>18.48751724630511</v>
+      </c>
+      <c r="BA6" s="34">
+        <f>PadRates!BA6*WellPressure!$Q$1</f>
+        <v>18.480338796369434</v>
+      </c>
       <c r="BB6" s="84"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
-      <c r="AD7" s="34"/>
-      <c r="AE7" s="34"/>
-      <c r="AF7" s="34"/>
-      <c r="AG7" s="34"/>
-      <c r="AH7" s="34"/>
-      <c r="AI7" s="34"/>
-      <c r="AJ7" s="34"/>
-      <c r="AK7" s="34"/>
-      <c r="AL7" s="34"/>
-      <c r="AM7" s="34"/>
-      <c r="AN7" s="34"/>
-      <c r="AO7" s="34"/>
-      <c r="AP7" s="34"/>
-      <c r="AQ7" s="34"/>
-      <c r="AR7" s="34"/>
-      <c r="AS7" s="34"/>
-      <c r="AT7" s="34"/>
-      <c r="AU7" s="34"/>
-      <c r="AV7" s="34"/>
-      <c r="AW7" s="34"/>
-      <c r="AX7" s="34"/>
-      <c r="AY7" s="34"/>
-      <c r="AZ7" s="34"/>
-      <c r="BA7" s="35"/>
+      <c r="A7" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="34">
+        <f>FlowbackRates!B3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="34">
+        <f>FlowbackRates!C3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="34">
+        <f>FlowbackRates!D3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="34">
+        <f>FlowbackRates!E3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="34">
+        <f>FlowbackRates!F3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="34">
+        <f>FlowbackRates!G3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="34">
+        <f>FlowbackRates!H3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="34">
+        <f>FlowbackRates!I3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="34">
+        <f>FlowbackRates!J3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="34">
+        <f>FlowbackRates!K3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="34">
+        <f>FlowbackRates!L3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="34">
+        <f>FlowbackRates!M3*WellPressure!$Q$1</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="34">
+        <f>FlowbackRates!N3*WellPressure!$Q$1</f>
+        <v>320</v>
+      </c>
+      <c r="O7" s="34">
+        <f>FlowbackRates!O3*WellPressure!$Q$1</f>
+        <v>251.06691132696025</v>
+      </c>
+      <c r="P7" s="34">
+        <f>FlowbackRates!P3*WellPressure!$Q$1</f>
+        <v>217.84998740750413</v>
+      </c>
+      <c r="Q7" s="34">
+        <f>FlowbackRates!Q3*WellPressure!$Q$1</f>
+        <v>196.9831061351866</v>
+      </c>
+      <c r="R7" s="34">
+        <f>FlowbackRates!R3*WellPressure!$Q$1</f>
+        <v>182.18410221604901</v>
+      </c>
+      <c r="S7" s="34">
+        <f>FlowbackRates!S3*WellPressure!$Q$1</f>
+        <v>170.92163584693515</v>
+      </c>
+      <c r="T7" s="34">
+        <f>FlowbackRates!T3*WellPressure!$Q$1</f>
+        <v>161.94429913758717</v>
+      </c>
+      <c r="U7" s="34">
+        <f>FlowbackRates!U3*WellPressure!$Q$1</f>
+        <v>154.54981262797531</v>
+      </c>
+      <c r="V7" s="34">
+        <f>FlowbackRates!V3*WellPressure!$Q$1</f>
+        <v>148.30817816703032</v>
+      </c>
+      <c r="W7" s="34">
+        <f>FlowbackRates!W3*WellPressure!$Q$1</f>
+        <v>142.93874948830822</v>
+      </c>
+      <c r="X7" s="34">
+        <f>FlowbackRates!X3*WellPressure!$Q$1</f>
+        <v>138.24917187280025</v>
+      </c>
+      <c r="Y7" s="34">
+        <f>FlowbackRates!Y3*WellPressure!$Q$1</f>
+        <v>134.10239747200455</v>
+      </c>
+      <c r="Z7" s="34">
+        <f>FlowbackRates!Z3*WellPressure!$Q$1</f>
+        <v>130.39766210409243</v>
+      </c>
+      <c r="AA7" s="34">
+        <f>FlowbackRates!AA3*WellPressure!$Q$1</f>
+        <v>127.05892184838537</v>
+      </c>
+      <c r="AB7" s="34">
+        <f>FlowbackRates!AB3*WellPressure!$Q$1</f>
+        <v>124.02751366754285</v>
+      </c>
+      <c r="AC7" s="34">
+        <f>FlowbackRates!AC3*WellPressure!$Q$1</f>
+        <v>121.25732532083187</v>
+      </c>
+      <c r="AD7" s="34">
+        <f>FlowbackRates!AD3*WellPressure!$Q$1</f>
+        <v>118.71151727884671</v>
+      </c>
+      <c r="AE7" s="34">
+        <f>FlowbackRates!AE3*WellPressure!$Q$1</f>
+        <v>116.3602381778901</v>
+      </c>
+      <c r="AF7" s="34">
+        <f>FlowbackRates!AF3*WellPressure!$Q$1</f>
+        <v>114.17899551150956</v>
+      </c>
+      <c r="AG7" s="34">
+        <f>FlowbackRates!AG3*WellPressure!$Q$1</f>
+        <v>112.14746982177395</v>
+      </c>
+      <c r="AH7" s="34">
+        <f>FlowbackRates!AH3*WellPressure!$Q$1</f>
+        <v>110.24863602450138</v>
+      </c>
+      <c r="AI7" s="34">
+        <f>FlowbackRates!AI3*WellPressure!$Q$1</f>
+        <v>108.46810179879381</v>
+      </c>
+      <c r="AJ7" s="34">
+        <f>FlowbackRates!AJ3*WellPressure!$Q$1</f>
+        <v>106.79360219799264</v>
+      </c>
+      <c r="AK7" s="34">
+        <f>FlowbackRates!AK3*WellPressure!$Q$1</f>
+        <v>105.21460854636418</v>
+      </c>
+      <c r="AL7" s="34">
+        <f>FlowbackRates!AL3*WellPressure!$Q$1</f>
+        <v>103.72202218833682</v>
+      </c>
+      <c r="AM7" s="34">
+        <f>FlowbackRates!AM3*WellPressure!$Q$1</f>
+        <v>102.30793208978467</v>
+      </c>
+      <c r="AN7" s="34">
+        <f>FlowbackRates!AN3*WellPressure!$Q$1</f>
+        <v>100.965421081617</v>
+      </c>
+      <c r="AO7" s="34">
+        <f>FlowbackRates!AO3*WellPressure!$Q$1</f>
+        <v>99.688409578149162</v>
+      </c>
+      <c r="AP7" s="34">
+        <f>FlowbackRates!AP3*WellPressure!$Q$1</f>
+        <v>98.471528467022637</v>
+      </c>
+      <c r="AQ7" s="34">
+        <f>FlowbackRates!AQ3*WellPressure!$Q$1</f>
+        <v>97.310014925226028</v>
+      </c>
+      <c r="AR7" s="34">
+        <f>FlowbackRates!AR3*WellPressure!$Q$1</f>
+        <v>96.199626413057672</v>
+      </c>
+      <c r="AS7" s="34">
+        <f>FlowbackRates!AS3*WellPressure!$Q$1</f>
+        <v>95.136569200217693</v>
+      </c>
+      <c r="AT7" s="34">
+        <f>FlowbackRates!AT3*WellPressure!$Q$1</f>
+        <v>94.117438598710649</v>
+      </c>
+      <c r="AU7" s="34">
+        <f>FlowbackRates!AU3*WellPressure!$Q$1</f>
+        <v>93.139168694178466</v>
+      </c>
+      <c r="AV7" s="34">
+        <f>FlowbackRates!AV3*WellPressure!$Q$1</f>
+        <v>92.19898983558933</v>
+      </c>
+      <c r="AW7" s="34">
+        <f>FlowbackRates!AW3*WellPressure!$Q$1</f>
+        <v>91.294392501850965</v>
+      </c>
+      <c r="AX7" s="34">
+        <f>FlowbackRates!AX3*WellPressure!$Q$1</f>
+        <v>90.423096440873636</v>
+      </c>
+      <c r="AY7" s="34">
+        <f>FlowbackRates!AY3*WellPressure!$Q$1</f>
+        <v>89.583024192154866</v>
+      </c>
+      <c r="AZ7" s="34">
+        <f>FlowbackRates!AZ3*WellPressure!$Q$1</f>
+        <v>88.772278272951624</v>
+      </c>
+      <c r="BA7" s="34">
+        <f>FlowbackRates!BA3*WellPressure!$Q$1</f>
+        <v>87.9891214415196</v>
+      </c>
       <c r="BB7" s="84"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
@@ -8918,7 +9726,9 @@
   </sheetPr>
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:P21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9944,11 +10754,11 @@
   </sheetPr>
   <dimension ref="A1:BH61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M14" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9968,21 +10778,51 @@
       <c r="A2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="116"/>
+      <c r="B2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="81" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" s="81" t="s">
+        <v>120</v>
+      </c>
+      <c r="O2" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="Q2" s="116"/>
       <c r="R2" s="116"/>
       <c r="S2" s="116"/>
@@ -10029,22 +10869,54 @@
       <c r="BH2" s="116"/>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="A3" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="78">
+        <v>0</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="78">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="78">
+        <v>0</v>
+      </c>
+      <c r="O3" s="92">
+        <v>0</v>
+      </c>
+      <c r="P3" s="29">
+        <v>0</v>
+      </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
@@ -10091,22 +10963,54 @@
       <c r="BH3" s="7"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="A4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="78">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="78">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4" s="78">
+        <v>0</v>
+      </c>
+      <c r="O4" s="92">
+        <v>0</v>
+      </c>
+      <c r="P4" s="29">
+        <v>0</v>
+      </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -10153,22 +11057,54 @@
       <c r="BH4" s="7"/>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="A5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>6</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="78">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="78">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="N5" s="78">
+        <v>0</v>
+      </c>
+      <c r="O5" s="92">
+        <v>0</v>
+      </c>
+      <c r="P5" s="29">
+        <v>0</v>
+      </c>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
@@ -10215,22 +11151,54 @@
       <c r="BH5" s="7"/>
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="A6" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="79">
+        <v>0</v>
+      </c>
+      <c r="C6" s="79">
+        <v>0</v>
+      </c>
+      <c r="D6" s="79">
+        <v>0</v>
+      </c>
+      <c r="E6" s="79">
+        <v>0</v>
+      </c>
+      <c r="F6" s="79">
+        <v>0</v>
+      </c>
+      <c r="G6" s="79">
+        <v>0</v>
+      </c>
+      <c r="H6" s="79">
+        <v>0</v>
+      </c>
+      <c r="I6" s="79">
+        <v>0</v>
+      </c>
+      <c r="J6" s="80">
+        <v>0</v>
+      </c>
+      <c r="K6" s="79">
+        <v>0</v>
+      </c>
+      <c r="L6" s="80">
+        <v>0</v>
+      </c>
+      <c r="M6" s="79">
+        <v>0</v>
+      </c>
+      <c r="N6" s="80">
+        <v>0</v>
+      </c>
+      <c r="O6" s="93">
+        <v>0</v>
+      </c>
+      <c r="P6" s="82">
+        <v>0</v>
+      </c>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -10277,22 +11245,54 @@
       <c r="BH6" s="7"/>
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="A7" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="79">
+        <v>0</v>
+      </c>
+      <c r="C7" s="79">
+        <v>0</v>
+      </c>
+      <c r="D7" s="79">
+        <v>0</v>
+      </c>
+      <c r="E7" s="79">
+        <v>0</v>
+      </c>
+      <c r="F7" s="79">
+        <v>0</v>
+      </c>
+      <c r="G7" s="79">
+        <v>0</v>
+      </c>
+      <c r="H7" s="79">
+        <v>0</v>
+      </c>
+      <c r="I7" s="79">
+        <v>6</v>
+      </c>
+      <c r="J7" s="80">
+        <v>0</v>
+      </c>
+      <c r="K7" s="79">
+        <v>0</v>
+      </c>
+      <c r="L7" s="80">
+        <v>0</v>
+      </c>
+      <c r="M7" s="79">
+        <v>0</v>
+      </c>
+      <c r="N7" s="80">
+        <v>0</v>
+      </c>
+      <c r="O7" s="93">
+        <v>0</v>
+      </c>
+      <c r="P7" s="82">
+        <v>0</v>
+      </c>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
@@ -10339,22 +11339,54 @@
       <c r="BH7" s="7"/>
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="A8" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0</v>
+      </c>
+      <c r="J8" s="78">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>8</v>
+      </c>
+      <c r="L8" s="78">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0</v>
+      </c>
+      <c r="N8" s="78">
+        <v>0</v>
+      </c>
+      <c r="O8" s="92">
+        <v>0</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0</v>
+      </c>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
@@ -10401,22 +11433,54 @@
       <c r="BH8" s="7"/>
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="A9" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="7">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>8</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="78">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="78">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0</v>
+      </c>
+      <c r="N9" s="78">
+        <v>0</v>
+      </c>
+      <c r="O9" s="92">
+        <v>0</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0</v>
+      </c>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
@@ -10463,22 +11527,54 @@
       <c r="BH9" s="7"/>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="A10" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+      <c r="J10" s="78">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="78">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7">
+        <v>0</v>
+      </c>
+      <c r="N10" s="78">
+        <v>0</v>
+      </c>
+      <c r="O10" s="92">
+        <v>0</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0</v>
+      </c>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
@@ -10525,22 +11621,54 @@
       <c r="BH10" s="7"/>
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="A11" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="78">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="78">
+        <v>8</v>
+      </c>
+      <c r="M11" s="7">
+        <v>0</v>
+      </c>
+      <c r="N11" s="78">
+        <v>0</v>
+      </c>
+      <c r="O11" s="92">
+        <v>0</v>
+      </c>
+      <c r="P11" s="29">
+        <v>0</v>
+      </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
@@ -10587,22 +11715,54 @@
       <c r="BH11" s="7"/>
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="A12" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>8</v>
+      </c>
+      <c r="J12" s="78">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="78">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0</v>
+      </c>
+      <c r="N12" s="78">
+        <v>0</v>
+      </c>
+      <c r="O12" s="92">
+        <v>0</v>
+      </c>
+      <c r="P12" s="29">
+        <v>0</v>
+      </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
@@ -10649,22 +11809,54 @@
       <c r="BH12" s="7"/>
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="A13" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="78">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="78">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>0</v>
+      </c>
+      <c r="N13" s="78">
+        <v>0</v>
+      </c>
+      <c r="O13" s="92">
+        <v>0</v>
+      </c>
+      <c r="P13" s="29">
+        <v>0</v>
+      </c>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
@@ -10711,22 +11903,54 @@
       <c r="BH13" s="7"/>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="A14" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>8</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <v>8</v>
+      </c>
+      <c r="J14" s="78">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14" s="78">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
+        <v>0</v>
+      </c>
+      <c r="N14" s="78">
+        <v>0</v>
+      </c>
+      <c r="O14" s="92">
+        <v>0</v>
+      </c>
+      <c r="P14" s="29">
+        <v>0</v>
+      </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
       <c r="S14" s="7"/>
@@ -10773,22 +11997,54 @@
       <c r="BH14" s="7"/>
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="A15" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>8</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="78">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="78">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
+      <c r="N15" s="78">
+        <v>0</v>
+      </c>
+      <c r="O15" s="92">
+        <v>0</v>
+      </c>
+      <c r="P15" s="29">
+        <v>0</v>
+      </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
@@ -10835,22 +12091,54 @@
       <c r="BH15" s="7"/>
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="A16" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="79">
+        <v>0</v>
+      </c>
+      <c r="C16" s="79">
+        <v>0</v>
+      </c>
+      <c r="D16" s="79">
+        <v>0</v>
+      </c>
+      <c r="E16" s="79">
+        <v>0</v>
+      </c>
+      <c r="F16" s="79">
+        <v>0</v>
+      </c>
+      <c r="G16" s="79">
+        <v>0</v>
+      </c>
+      <c r="H16" s="79">
+        <v>0</v>
+      </c>
+      <c r="I16" s="79">
+        <v>0</v>
+      </c>
+      <c r="J16" s="80">
+        <v>0</v>
+      </c>
+      <c r="K16" s="79">
+        <v>0</v>
+      </c>
+      <c r="L16" s="80">
+        <v>0</v>
+      </c>
+      <c r="M16" s="79">
+        <v>0</v>
+      </c>
+      <c r="N16" s="80">
+        <v>0</v>
+      </c>
+      <c r="O16" s="93">
+        <v>0</v>
+      </c>
+      <c r="P16" s="82">
+        <v>0</v>
+      </c>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
@@ -10897,22 +12185,54 @@
       <c r="BH16" s="7"/>
     </row>
     <row r="17" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="A17" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="79">
+        <v>0</v>
+      </c>
+      <c r="C17" s="79">
+        <v>0</v>
+      </c>
+      <c r="D17" s="79">
+        <v>0</v>
+      </c>
+      <c r="E17" s="79">
+        <v>0</v>
+      </c>
+      <c r="F17" s="79">
+        <v>0</v>
+      </c>
+      <c r="G17" s="79">
+        <v>0</v>
+      </c>
+      <c r="H17" s="79">
+        <v>0</v>
+      </c>
+      <c r="I17" s="79">
+        <v>0</v>
+      </c>
+      <c r="J17" s="80">
+        <v>0</v>
+      </c>
+      <c r="K17" s="79">
+        <v>0</v>
+      </c>
+      <c r="L17" s="80">
+        <v>0</v>
+      </c>
+      <c r="M17" s="79">
+        <v>0</v>
+      </c>
+      <c r="N17" s="80">
+        <v>0</v>
+      </c>
+      <c r="O17" s="93">
+        <v>0</v>
+      </c>
+      <c r="P17" s="82">
+        <v>0</v>
+      </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
@@ -10959,22 +12279,54 @@
       <c r="BH17" s="7"/>
     </row>
     <row r="18" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="A18" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0</v>
+      </c>
+      <c r="J18" s="78">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="78">
+        <v>0</v>
+      </c>
+      <c r="M18" s="7">
+        <v>0</v>
+      </c>
+      <c r="N18" s="78">
+        <v>0</v>
+      </c>
+      <c r="O18" s="92">
+        <v>0</v>
+      </c>
+      <c r="P18" s="29">
+        <v>8</v>
+      </c>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
@@ -11021,22 +12373,54 @@
       <c r="BH18" s="7"/>
     </row>
     <row r="19" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="A19" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="79">
+        <v>0</v>
+      </c>
+      <c r="C19" s="79">
+        <v>0</v>
+      </c>
+      <c r="D19" s="79">
+        <v>0</v>
+      </c>
+      <c r="E19" s="79">
+        <v>0</v>
+      </c>
+      <c r="F19" s="79">
+        <v>0</v>
+      </c>
+      <c r="G19" s="79">
+        <v>0</v>
+      </c>
+      <c r="H19" s="79">
+        <v>0</v>
+      </c>
+      <c r="I19" s="79">
+        <v>0</v>
+      </c>
+      <c r="J19" s="80">
+        <v>0</v>
+      </c>
+      <c r="K19" s="79">
+        <v>0</v>
+      </c>
+      <c r="L19" s="80">
+        <v>0</v>
+      </c>
+      <c r="M19" s="79">
+        <v>0</v>
+      </c>
+      <c r="N19" s="80">
+        <v>0</v>
+      </c>
+      <c r="O19" s="93">
+        <v>0</v>
+      </c>
+      <c r="P19" s="82">
+        <v>8</v>
+      </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
       <c r="S19" s="7"/>
@@ -11083,22 +12467,54 @@
       <c r="BH19" s="7"/>
     </row>
     <row r="20" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="A20" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7">
+        <v>0</v>
+      </c>
+      <c r="J20" s="78">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="78">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0</v>
+      </c>
+      <c r="N20" s="78">
+        <v>0</v>
+      </c>
+      <c r="O20" s="92">
+        <v>0</v>
+      </c>
+      <c r="P20" s="29">
+        <v>0</v>
+      </c>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
@@ -11144,23 +12560,55 @@
       <c r="BG20" s="7"/>
       <c r="BH20" s="7"/>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+    <row r="21" spans="1:60" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="83">
+        <v>0</v>
+      </c>
+      <c r="K21" s="8">
+        <v>0</v>
+      </c>
+      <c r="L21" s="83">
+        <v>0</v>
+      </c>
+      <c r="M21" s="8">
+        <v>0</v>
+      </c>
+      <c r="N21" s="83">
+        <v>0</v>
+      </c>
+      <c r="O21" s="94">
+        <v>8</v>
+      </c>
+      <c r="P21" s="9">
+        <v>0</v>
+      </c>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
       <c r="S21" s="7"/>

</xml_diff>

<commit_message>
Remove links in input file
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7738F090-7E23-435A-BF5C-A1D1836FAE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D6801-1A59-4A6E-8DF8-E9ABDBC9378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="73" activeTab="79" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="72" activeTab="79" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId85"/>
     <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId86"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId87"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="70" hidden="1">#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="70">PipelineExpansionDistance!#REF!</definedName>
@@ -2057,254 +2054,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Overview"/>
-      <sheetName val="Schematic"/>
-      <sheetName val="Units"/>
-      <sheetName val="ProductionPads"/>
-      <sheetName val="ProductionTanks"/>
-      <sheetName val="CompletionsPads"/>
-      <sheetName val="SWDSites"/>
-      <sheetName val="FreshwaterSources"/>
-      <sheetName val="StorageSites"/>
-      <sheetName val="TreatmentSites"/>
-      <sheetName val="TreatmentTechnologies"/>
-      <sheetName val="ReuseOptions"/>
-      <sheetName val="NetworkNodes"/>
-      <sheetName val="PipelineDiameters"/>
-      <sheetName val="StorageCapacities"/>
-      <sheetName val="TreatmentCapacities"/>
-      <sheetName val="InjectionCapacities"/>
-      <sheetName val="PNA"/>
-      <sheetName val="CNA"/>
-      <sheetName val="CCA"/>
-      <sheetName val="NNA"/>
-      <sheetName val="NCA"/>
-      <sheetName val="NKA"/>
-      <sheetName val="NRA"/>
-      <sheetName val="NSA"/>
-      <sheetName val="NOA"/>
-      <sheetName val="SNA"/>
-      <sheetName val="SOA"/>
-      <sheetName val="FCA"/>
-      <sheetName val="RCA"/>
-      <sheetName val="RSA"/>
-      <sheetName val="SCA"/>
-      <sheetName val="RNA"/>
-      <sheetName val="ROA"/>
-      <sheetName val="PCT"/>
-      <sheetName val="FCT"/>
-      <sheetName val="PKT"/>
-      <sheetName val="CKT"/>
-      <sheetName val="CCT"/>
-      <sheetName val="CST"/>
-      <sheetName val="RST"/>
-      <sheetName val="ROT"/>
-      <sheetName val="SOT"/>
-      <sheetName val="CompletionsDemand"/>
-      <sheetName val="PadRates"/>
-      <sheetName val="FlowbackRates"/>
-      <sheetName val="InitialPipelineCapacity"/>
-      <sheetName val="InitialDisposalCapacity"/>
-      <sheetName val="InitialStorageCapacity"/>
-      <sheetName val="InitialTreatmentCapacity"/>
-      <sheetName val="ReuseCapacity"/>
-      <sheetName val="FreshwaterSourcingAvailability"/>
-      <sheetName val="CompletionsPadStorage"/>
-      <sheetName val="PadOffloadingCapacity"/>
-      <sheetName val="NodeCapacities"/>
-      <sheetName val="DisposalOperatingCapacity"/>
-      <sheetName val="DisposalOperationalCost"/>
-      <sheetName val="TreatmentOperationalCost"/>
-      <sheetName val="ReuseOperationalCost"/>
-      <sheetName val="PipelineOperationalCost"/>
-      <sheetName val="FreshSourcingCost"/>
-      <sheetName val="TruckingHourlyCost"/>
-      <sheetName val="TruckingTime"/>
-      <sheetName val="DisposalExpansionCost"/>
-      <sheetName val="DisposalCapacityIncrements"/>
-      <sheetName val="StorageExpansionCost"/>
-      <sheetName val="StorageCapacityIncrements"/>
-      <sheetName val="TreatmentExpansionCost"/>
-      <sheetName val="TreatmentCapacityIncrements"/>
-      <sheetName val="PipelineCapexDistanceBased"/>
-      <sheetName val="PipelineExpansionDistance"/>
-      <sheetName val="PipelineCapexCapacityBased"/>
-      <sheetName val="PipelineCapacityIncrements"/>
-      <sheetName val="PipelineDiameterValues"/>
-      <sheetName val="TreatmentEfficiency"/>
-      <sheetName val="RemovalEfficiency"/>
-      <sheetName val="DesalinationTechnologies"/>
-      <sheetName val="DesalinationSites"/>
-      <sheetName val="DesalinationBrineReuse"/>
-      <sheetName val="BeneficialReuseCredit"/>
-      <sheetName val="CompletionsPadOutsideSystem"/>
-      <sheetName val="Hydraulics"/>
-      <sheetName val="Economics"/>
-      <sheetName val="PadWaterQuality"/>
-      <sheetName val="StorageInitialWaterQuality"/>
-      <sheetName val="PadStorageInitialWaterQuality"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>INDEX</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>VALUE</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>volume</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>bbl</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>distance</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>mile</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>diameter</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>inch</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>concentration</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>mg/liter</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>currency</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>USD</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>time</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>day</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>decision period</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>week</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-      <sheetData sheetId="85"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9276,8 +9025,8 @@
   <sheetData>
     <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Beneficial Reuse Capacity [",VLOOKUP("volume", [1]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [1]Units!$A$2:$B$9, 2, FALSE),"]. Use a negative number to denote no upper limit for capacity at a given reuse site and time.")</f>
-        <v>Table of Beneficial Reuse Capacity [bbl/day]. Use a negative number to denote no upper limit for capacity at a given reuse site and time.</v>
+        <f>_xlfn.CONCAT( "Table of Beneficial Reuse Capacity [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Beneficial Reuse Capacity [bbl/day]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -15286,7 +15035,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", [1]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", [1]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove DesalinationBrineReuse tab from input file
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D6801-1A59-4A6E-8DF8-E9ABDBC9378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EBD9DE-8CFC-4B34-B631-7F401FAC3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="72" activeTab="79" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="16" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -91,14 +91,13 @@
     <sheet name="RemovalEfficiency" sheetId="114" r:id="rId76"/>
     <sheet name="DesalinationTechnologies" sheetId="111" r:id="rId77"/>
     <sheet name="DesalinationSites" sheetId="113" r:id="rId78"/>
-    <sheet name="DesalinationBrineReuse" sheetId="123" r:id="rId79"/>
-    <sheet name="BeneficialReuseCredit" sheetId="125" r:id="rId80"/>
-    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId81"/>
-    <sheet name="Hydraulics" sheetId="93" r:id="rId82"/>
-    <sheet name="Economics" sheetId="95" r:id="rId83"/>
-    <sheet name="PadWaterQuality" sheetId="99" r:id="rId84"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId85"/>
-    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId86"/>
+    <sheet name="BeneficialReuseCredit" sheetId="125" r:id="rId79"/>
+    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId80"/>
+    <sheet name="Hydraulics" sheetId="93" r:id="rId81"/>
+    <sheet name="Economics" sheetId="95" r:id="rId82"/>
+    <sheet name="PadWaterQuality" sheetId="99" r:id="rId83"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId84"/>
+    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId85"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="70" hidden="1">#REF!</definedName>
@@ -125,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="271">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -916,31 +915,28 @@
     <t>Storage Sites to Beneficial Reuse Piping Arcs [-]</t>
   </si>
   <si>
-    <t>Treatment Sites to Beneficial Reuse Piping Arcs (for desalination sites with reusable brine, 2 denotes an arc for the brine stream) [-]</t>
-  </si>
-  <si>
-    <t>Treatment Sites to Completions Sites Piping Arcs (for desalination sites with reusable brine, 2 denotes an arc for the brine stream) [-]</t>
-  </si>
-  <si>
-    <t>Treatment Sites to Storage Sites Piping Arcs (for desalination sites with reusable brine, 2 denotes an arc for the brine stream) [-]</t>
-  </si>
-  <si>
-    <t>Treatment Sites to Network Nodes Piping Arcs (for desalination sites with reusable brine, 2 denotes an arc for the brine stream) [-]</t>
-  </si>
-  <si>
-    <t>Treatment Sites to Storage Sites Trucking Arcs (for desalination sites with reusable brine, 2 denotes an arc for the brine stream) [-]</t>
-  </si>
-  <si>
-    <t>Treatment Sites to Beneficial Reuse Trucking Arcs (for desalination sites with reusable brine, 2 denotes an arc for the brine stream) [-]</t>
-  </si>
-  <si>
     <t>Storage Sites to Beneficial Reuse Trucking Arcs [-]</t>
   </si>
   <si>
-    <t>Table with indication for each desalination site whether or not the brine is reused (1 for yes, 0 for no)</t>
-  </si>
-  <si>
     <t>ReuseOptions</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Completions Sites Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Storage Sites Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Network Nodes Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Beneficial Reuse Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Storage Sites Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Treatment Sites to Beneficial Reuse Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
 </sst>
 </file>
@@ -5051,7 +5047,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5099,7 +5095,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -5189,7 +5185,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5265,7 +5261,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5276,7 +5272,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -5736,7 +5732,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -5772,7 +5768,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -5783,7 +5779,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -5837,7 +5833,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -9036,7 +9032,7 @@
     </row>
     <row r="2" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>178</v>
@@ -14927,40 +14923,49 @@
 </file>
 
 <file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9102DFE-B382-4759-82AF-1C3ECC65F935}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704B3E-8A1A-4064-9703-FD38B5DAA6B6}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>270</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>169</v>
+        <v>264</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="33">
-        <v>1</v>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="33">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -15018,57 +15023,6 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704B3E-8A1A-4064-9703-FD38B5DAA6B6}">
-  <sheetPr>
-    <tabColor rgb="FFAFF3DE"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="B3" s="32">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="B4" s="33">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2338A37-BF8E-46F2-AA7C-FB95F874D0FC}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -15108,7 +15062,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDDE38-2D71-4494-ABC1-8D5269A138D9}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -15158,7 +15112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -15208,7 +15162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134045F2-617D-4B6C-9AE3-C6E73CF3B321}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -15291,7 +15245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE4BAFD-2A94-4164-976F-B9E5B42E5AAB}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -15333,7 +15287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA334136-9628-4654-B8E2-BCFE701B0D1B}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>

</xml_diff>

<commit_message>
Add beneficial reuse minimum tab and constraint
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EBD9DE-8CFC-4B34-B631-7F401FAC3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B5D913-E8C9-4829-B7A2-2809B4EB0B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="16" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" firstSheet="40" activeTab="50" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -63,45 +63,46 @@
     <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId48"/>
     <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId49"/>
     <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId50"/>
-    <sheet name="ReuseCapacity" sheetId="124" r:id="rId51"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId52"/>
-    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId53"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId54"/>
-    <sheet name="NodeCapacities" sheetId="102" r:id="rId55"/>
-    <sheet name="DisposalOperatingCapacity" sheetId="112" r:id="rId56"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId57"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId58"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId59"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId60"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId61"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId62"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId63"/>
-    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId64"/>
-    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId65"/>
-    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId66"/>
-    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId67"/>
-    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId68"/>
-    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId69"/>
-    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId70"/>
-    <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId71"/>
-    <sheet name="PipelineCapexCapacityBased" sheetId="98" r:id="rId72"/>
-    <sheet name="PipelineCapacityIncrements" sheetId="97" r:id="rId73"/>
-    <sheet name="PipelineDiameterValues" sheetId="78" r:id="rId74"/>
-    <sheet name="TreatmentEfficiency" sheetId="107" r:id="rId75"/>
-    <sheet name="RemovalEfficiency" sheetId="114" r:id="rId76"/>
-    <sheet name="DesalinationTechnologies" sheetId="111" r:id="rId77"/>
-    <sheet name="DesalinationSites" sheetId="113" r:id="rId78"/>
-    <sheet name="BeneficialReuseCredit" sheetId="125" r:id="rId79"/>
-    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId80"/>
-    <sheet name="Hydraulics" sheetId="93" r:id="rId81"/>
-    <sheet name="Economics" sheetId="95" r:id="rId82"/>
-    <sheet name="PadWaterQuality" sheetId="99" r:id="rId83"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId84"/>
-    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId85"/>
+    <sheet name="ReuseMinimum" sheetId="126" r:id="rId51"/>
+    <sheet name="ReuseCapacity" sheetId="124" r:id="rId52"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId53"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId54"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId55"/>
+    <sheet name="NodeCapacities" sheetId="102" r:id="rId56"/>
+    <sheet name="DisposalOperatingCapacity" sheetId="112" r:id="rId57"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId58"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId59"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId60"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId61"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId62"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId63"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId64"/>
+    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId65"/>
+    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId66"/>
+    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId67"/>
+    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId68"/>
+    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId69"/>
+    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId70"/>
+    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId71"/>
+    <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId72"/>
+    <sheet name="PipelineCapexCapacityBased" sheetId="98" r:id="rId73"/>
+    <sheet name="PipelineCapacityIncrements" sheetId="97" r:id="rId74"/>
+    <sheet name="PipelineDiameterValues" sheetId="78" r:id="rId75"/>
+    <sheet name="TreatmentEfficiency" sheetId="107" r:id="rId76"/>
+    <sheet name="RemovalEfficiency" sheetId="114" r:id="rId77"/>
+    <sheet name="DesalinationTechnologies" sheetId="111" r:id="rId78"/>
+    <sheet name="DesalinationSites" sheetId="113" r:id="rId79"/>
+    <sheet name="BeneficialReuseCredit" sheetId="125" r:id="rId80"/>
+    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId81"/>
+    <sheet name="Hydraulics" sheetId="93" r:id="rId82"/>
+    <sheet name="Economics" sheetId="95" r:id="rId83"/>
+    <sheet name="PadWaterQuality" sheetId="99" r:id="rId84"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId85"/>
+    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId86"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="70" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="70">PipelineExpansionDistance!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="71" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="71">PipelineExpansionDistance!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -124,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="271">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1626,7 +1627,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1924,6 +1925,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5768,7 +5772,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -9003,6 +9007,522 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D82FC29-1A28-47CD-9CF9-58F230312687}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:BA4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="53" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Beneficial Reuse minimum required flow [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Beneficial Reuse minimum required flow [bbl/day]</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AO2" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="AP2" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AY2" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="AZ2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="BA2" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="119">
+        <v>0</v>
+      </c>
+      <c r="C3" s="119">
+        <v>0</v>
+      </c>
+      <c r="D3" s="119">
+        <v>0</v>
+      </c>
+      <c r="E3" s="119">
+        <v>0</v>
+      </c>
+      <c r="F3" s="119">
+        <v>0</v>
+      </c>
+      <c r="G3" s="119">
+        <v>0</v>
+      </c>
+      <c r="H3" s="119">
+        <v>0</v>
+      </c>
+      <c r="I3" s="119">
+        <v>0</v>
+      </c>
+      <c r="J3" s="119">
+        <v>0</v>
+      </c>
+      <c r="K3" s="119">
+        <v>0</v>
+      </c>
+      <c r="L3" s="119">
+        <v>0</v>
+      </c>
+      <c r="M3" s="119">
+        <v>0</v>
+      </c>
+      <c r="N3" s="119">
+        <v>0</v>
+      </c>
+      <c r="O3" s="119">
+        <v>0</v>
+      </c>
+      <c r="P3" s="119">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="119">
+        <v>0</v>
+      </c>
+      <c r="R3" s="119">
+        <v>0</v>
+      </c>
+      <c r="S3" s="119">
+        <v>0</v>
+      </c>
+      <c r="T3" s="119">
+        <v>0</v>
+      </c>
+      <c r="U3" s="119">
+        <v>0</v>
+      </c>
+      <c r="V3" s="119">
+        <v>0</v>
+      </c>
+      <c r="W3" s="119">
+        <v>0</v>
+      </c>
+      <c r="X3" s="119">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="119">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="119">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="119">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="36">
+        <v>0</v>
+      </c>
+      <c r="C4" s="36">
+        <v>0</v>
+      </c>
+      <c r="D4" s="36">
+        <v>0</v>
+      </c>
+      <c r="E4" s="36">
+        <v>0</v>
+      </c>
+      <c r="F4" s="36">
+        <v>0</v>
+      </c>
+      <c r="G4" s="36">
+        <v>0</v>
+      </c>
+      <c r="H4" s="36">
+        <v>0</v>
+      </c>
+      <c r="I4" s="36">
+        <v>0</v>
+      </c>
+      <c r="J4" s="36">
+        <v>0</v>
+      </c>
+      <c r="K4" s="36">
+        <v>0</v>
+      </c>
+      <c r="L4" s="36">
+        <v>0</v>
+      </c>
+      <c r="M4" s="36">
+        <v>0</v>
+      </c>
+      <c r="N4" s="36">
+        <v>0</v>
+      </c>
+      <c r="O4" s="36">
+        <v>0</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>0</v>
+      </c>
+      <c r="R4" s="36">
+        <v>0</v>
+      </c>
+      <c r="S4" s="36">
+        <v>0</v>
+      </c>
+      <c r="T4" s="36">
+        <v>0</v>
+      </c>
+      <c r="U4" s="36">
+        <v>0</v>
+      </c>
+      <c r="V4" s="36">
+        <v>0</v>
+      </c>
+      <c r="W4" s="36">
+        <v>0</v>
+      </c>
+      <c r="X4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="36">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="37">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83B7EA2-F58B-4387-ADEC-3EDB6AA19817}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -9010,7 +9530,7 @@
   <dimension ref="A1:BA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9518,7 +10038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -10156,7 +10676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -10200,7 +10720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -10243,7 +10763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF13C221-12DF-4609-BB39-C92B41E7288D}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -10337,7 +10857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938F1661-765C-4FF3-9C8D-056B836A43E1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -10858,7 +11378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -10910,7 +11430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -11053,49 +11573,6 @@
       </c>
       <c r="C12" s="33">
         <v>0.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Reuse Operational Cost [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11153,6 +11630,49 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Reuse Operational Cost [USD/bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12303,7 +12823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12354,7 +12874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12445,7 +12965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12536,7 +13056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12615,7 +13135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12684,7 +13204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344AC655-401B-435E-9F3E-B4AFCEDA07DB}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12745,7 +13265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F26805-7F3D-4935-8D0C-80B2E9E9F409}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -12814,7 +13334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D3944-A6F1-468B-A756-A99C077811C6}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -13057,145 +13577,6 @@
       <c r="F12" s="37">
         <v>800</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6DB070-53D7-4763-B1D6-04233A007F0E}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Treatment Capacity Expansion Increments [bbl/day]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="34">
-        <v>0</v>
-      </c>
-      <c r="C3" s="34">
-        <v>10000</v>
-      </c>
-      <c r="D3" s="34">
-        <v>20000</v>
-      </c>
-      <c r="E3" s="35">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="34">
-        <v>0</v>
-      </c>
-      <c r="C4" s="34">
-        <v>10000</v>
-      </c>
-      <c r="D4" s="34">
-        <v>20000</v>
-      </c>
-      <c r="E4" s="35">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="B5" s="34">
-        <v>0</v>
-      </c>
-      <c r="C5" s="34">
-        <v>10000</v>
-      </c>
-      <c r="D5" s="34">
-        <v>20000</v>
-      </c>
-      <c r="E5" s="35">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="B6" s="34">
-        <v>0</v>
-      </c>
-      <c r="C6" s="34">
-        <v>10000</v>
-      </c>
-      <c r="D6" s="34">
-        <v>20000</v>
-      </c>
-      <c r="E6" s="35">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="B7" s="36">
-        <v>0</v>
-      </c>
-      <c r="C7" s="36">
-        <v>10000</v>
-      </c>
-      <c r="D7" s="36">
-        <v>20000</v>
-      </c>
-      <c r="E7" s="37">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="75"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13254,6 +13635,145 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6DB070-53D7-4763-B1D6-04233A007F0E}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Treatment Capacity Expansion Increments [bbl/day]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="34">
+        <v>0</v>
+      </c>
+      <c r="C3" s="34">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="34">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="35">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="34">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="34">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="35">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" s="34">
+        <v>0</v>
+      </c>
+      <c r="C5" s="34">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="34">
+        <v>20000</v>
+      </c>
+      <c r="E5" s="35">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="34">
+        <v>0</v>
+      </c>
+      <c r="C6" s="34">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="34">
+        <v>20000</v>
+      </c>
+      <c r="E6" s="35">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" s="36">
+        <v>0</v>
+      </c>
+      <c r="C7" s="36">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="36">
+        <v>20000</v>
+      </c>
+      <c r="E7" s="37">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="75"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="75"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C902C13-E391-4A34-8851-63FF84EE5034}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -13297,7 +13817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE67BAE-6607-47A3-AB16-0544FAF51C24}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -14259,7 +14779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD7B182-CFB4-4537-B5F7-69962DD30DA1}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -14354,7 +14874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BBCD48-6980-4EA6-BF3E-79D1C64EA04C}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -14431,7 +14951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805632D3-BD42-4D5C-8C0F-68DF124ED3E8}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -14508,7 +15028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D674F75E-153D-40A1-94D4-31ED20AACD7B}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -14654,7 +15174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FD92FF-3AD4-4D23-8578-311AD898F13B}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -14802,7 +15322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5996B071-C07A-46F0-B343-7584DB2F1269}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -14874,7 +15394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE80B7E4-4C81-4B91-B37B-915E590A92F2}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -14915,57 +15435,6 @@
       </c>
       <c r="B4" s="33">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704B3E-8A1A-4064-9703-FD38B5DAA6B6}">
-  <sheetPr>
-    <tabColor rgb="FFAFF3DE"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="B3" s="32">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="B4" s="33">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -15023,6 +15492,57 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D704B3E-8A1A-4064-9703-FD38B5DAA6B6}">
+  <sheetPr>
+    <tabColor rgb="FFAFF3DE"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" s="32">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="33">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2338A37-BF8E-46F2-AA7C-FB95F874D0FC}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -15062,7 +15582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDDE38-2D71-4494-ABC1-8D5269A138D9}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -15112,7 +15632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -15162,7 +15682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134045F2-617D-4B6C-9AE3-C6E73CF3B321}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -15245,7 +15765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE4BAFD-2A94-4164-976F-B9E5B42E5AAB}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -15287,7 +15807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA334136-9628-4654-B8E2-BCFE701B0D1B}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>

</xml_diff>

<commit_message>
Update Elevation tab for toy case study, update schematic
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DB89BF-A3CB-410A-BA93-13B522A0E046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6E6D7D-2B25-4409-B705-75A83D5C1C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="289">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -2035,17 +2035,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>144425</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>39089</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>30363</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95848</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1471AA2-E63B-4D6A-BE14-72AE3450CF58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A07C3C-97EC-3104-F046-95ABEEA2623E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2062,7 +2062,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11107700" cy="7087589"/>
+          <a:ext cx="12812913" cy="4286848"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3714,7 +3714,9 @@
   </sheetPr>
   <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3829,7 +3831,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5906,7 +5908,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -5918,26 +5920,35 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="73" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6146,10 +6157,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6261,7 +6272,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="103" t="s">
-        <v>119</v>
+        <v>276</v>
       </c>
       <c r="B13" s="104">
         <v>500</v>
@@ -6269,81 +6280,121 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="103" t="s">
-        <v>120</v>
+        <v>277</v>
       </c>
       <c r="B14" s="104">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="103" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B15" s="104">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="103" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B16" s="104">
-        <v>600</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="103" t="s">
-        <v>127</v>
+        <v>278</v>
       </c>
       <c r="B17" s="104">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="103" t="s">
-        <v>128</v>
+        <v>279</v>
       </c>
       <c r="B18" s="104">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="103" t="s">
-        <v>129</v>
+        <v>280</v>
       </c>
       <c r="B19" s="104">
-        <v>550</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="103" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B20" s="104">
-        <v>550</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="103" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B21" s="104">
-        <v>550</v>
+        <v>600</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="103" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="104">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="103" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="104">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="104">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="103" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="104">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="103" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="104">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="103" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="104">
+      <c r="B27" s="104">
         <v>550</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="112" t="s">
+    <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="113">
+      <c r="B28" s="113">
         <v>500</v>
       </c>
     </row>
@@ -9860,7 +9911,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23177,7 +23228,7 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add new required tabs to Permian demo input file
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6E6D7D-2B25-4409-B705-75A83D5C1C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AFD480-8AA8-4DB8-A1A2-E46A9DD8875B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" firstSheet="28" activeTab="47" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1656,7 +1656,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1948,6 +1948,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2376,7 +2386,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6160,7 +6170,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6215,18 +6225,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="121" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="104">
+      <c r="B6" s="122">
         <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="104">
+      <c r="B7" s="124">
         <v>650</v>
       </c>
     </row>
@@ -6239,10 +6249,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="121" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="104">
+      <c r="B9" s="122">
         <v>600</v>
       </c>
     </row>
@@ -6255,10 +6265,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="104">
+      <c r="B11" s="122">
         <v>650</v>
       </c>
     </row>
@@ -6279,10 +6289,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="103" t="s">
+      <c r="A14" s="121" t="s">
         <v>277</v>
       </c>
-      <c r="B14" s="104">
+      <c r="B14" s="122">
         <v>500</v>
       </c>
     </row>
@@ -6295,10 +6305,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="121" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="104">
+      <c r="B16" s="122">
         <v>250</v>
       </c>
     </row>
@@ -6319,10 +6329,10 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="103" t="s">
+      <c r="A19" s="121" t="s">
         <v>280</v>
       </c>
-      <c r="B19" s="104">
+      <c r="B19" s="122">
         <v>500</v>
       </c>
     </row>
@@ -8211,7 +8221,7 @@
   </sheetPr>
   <dimension ref="A1:BC23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -8892,163 +8902,163 @@
       <c r="BB5" s="83"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="125">
         <v>20</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="125">
         <v>19.724654089867183</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="125">
         <v>19.565347714583421</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="125">
         <v>19.45309894824571</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="125">
         <v>19.366475714512596</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="125">
         <v>19.29598579090657</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="125">
         <v>19.236587614095988</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="125">
         <v>19.185282386505289</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="125">
         <v>19.14014155962774</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="125">
         <v>19.099851720428717</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="125">
         <v>19.063478193082773</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="125">
         <v>19.030332252431219</v>
       </c>
-      <c r="N6" s="34">
+      <c r="N6" s="125">
         <v>18.999891837835946</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="125">
         <v>18.971751827873344</v>
       </c>
-      <c r="P6" s="34">
+      <c r="P6" s="125">
         <v>18.945591568023726</v>
       </c>
-      <c r="Q6" s="34">
+      <c r="Q6" s="125">
         <v>18.92115293451192</v>
       </c>
-      <c r="R6" s="34">
+      <c r="R6" s="125">
         <v>18.898225082424748</v>
       </c>
-      <c r="S6" s="34">
+      <c r="S6" s="125">
         <v>18.876633574737408</v>
       </c>
-      <c r="T6" s="34">
+      <c r="T6" s="125">
         <v>18.856232464552253</v>
       </c>
-      <c r="U6" s="34">
+      <c r="U6" s="125">
         <v>18.836898417660557</v>
       </c>
-      <c r="V6" s="34">
+      <c r="V6" s="125">
         <v>18.818526275591836</v>
       </c>
-      <c r="W6" s="34">
+      <c r="W6" s="125">
         <v>18.8010256554142</v>
       </c>
-      <c r="X6" s="34">
+      <c r="X6" s="125">
         <v>18.784318308654296</v>
       </c>
-      <c r="Y6" s="34">
+      <c r="Y6" s="125">
         <v>18.768336044722442</v>
       </c>
-      <c r="Z6" s="34">
+      <c r="Z6" s="125">
         <v>18.75301908004031</v>
       </c>
-      <c r="AA6" s="34">
+      <c r="AA6" s="125">
         <v>18.738314712310245</v>
       </c>
-      <c r="AB6" s="34">
+      <c r="AB6" s="125">
         <v>18.724176246023287</v>
       </c>
-      <c r="AC6" s="34">
+      <c r="AC6" s="125">
         <v>18.710562114180359</v>
       </c>
-      <c r="AD6" s="34">
+      <c r="AD6" s="125">
         <v>18.697435154762537</v>
       </c>
-      <c r="AE6" s="34">
+      <c r="AE6" s="125">
         <v>18.684762010358615</v>
       </c>
-      <c r="AF6" s="34">
+      <c r="AF6" s="125">
         <v>18.672512626632653</v>
       </c>
-      <c r="AG6" s="34">
+      <c r="AG6" s="125">
         <v>18.660659830736151</v>
       </c>
-      <c r="AH6" s="34">
+      <c r="AH6" s="125">
         <v>18.649178974852152</v>
       </c>
-      <c r="AI6" s="34">
+      <c r="AI6" s="125">
         <v>18.638047633163993</v>
       </c>
-      <c r="AJ6" s="34">
+      <c r="AJ6" s="125">
         <v>18.627245342924191</v>
       </c>
-      <c r="AK6" s="34">
+      <c r="AK6" s="125">
         <v>18.616753382143422</v>
       </c>
-      <c r="AL6" s="34">
+      <c r="AL6" s="125">
         <v>18.606554577858702</v>
       </c>
-      <c r="AM6" s="34">
+      <c r="AM6" s="125">
         <v>18.59663314007085</v>
       </c>
-      <c r="AN6" s="34">
+      <c r="AN6" s="125">
         <v>18.586974517336788</v>
       </c>
-      <c r="AO6" s="34">
+      <c r="AO6" s="125">
         <v>18.577565270716047</v>
       </c>
-      <c r="AP6" s="34">
+      <c r="AP6" s="125">
         <v>18.568392963342752</v>
       </c>
-      <c r="AQ6" s="34">
+      <c r="AQ6" s="125">
         <v>18.559446063356276</v>
       </c>
-      <c r="AR6" s="34">
+      <c r="AR6" s="125">
         <v>18.550713858298163</v>
       </c>
-      <c r="AS6" s="34">
+      <c r="AS6" s="125">
         <v>18.54218637938818</v>
       </c>
-      <c r="AT6" s="34">
+      <c r="AT6" s="125">
         <v>18.533854334343193</v>
       </c>
-      <c r="AU6" s="34">
+      <c r="AU6" s="125">
         <v>18.525709047608249</v>
       </c>
-      <c r="AV6" s="34">
+      <c r="AV6" s="125">
         <v>18.517742407040306</v>
       </c>
-      <c r="AW6" s="34">
+      <c r="AW6" s="125">
         <v>18.509946816226808</v>
       </c>
-      <c r="AX6" s="34">
+      <c r="AX6" s="125">
         <v>18.502315151739563</v>
       </c>
-      <c r="AY6" s="34">
+      <c r="AY6" s="125">
         <v>18.494840724723719</v>
       </c>
-      <c r="AZ6" s="34">
+      <c r="AZ6" s="125">
         <v>18.48751724630511</v>
       </c>
-      <c r="BA6" s="35">
+      <c r="BA6" s="126">
         <v>18.480338796369434</v>
       </c>
       <c r="BB6" s="83"/>

</xml_diff>

<commit_message>
Add beneficial reuse tabs to small strategic case study input file
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AFD480-8AA8-4DB8-A1A2-E46A9DD8875B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF630C0-E3B6-406C-9426-9126D538B50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" firstSheet="28" activeTab="47" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2386,7 +2386,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8221,7 +8221,7 @@
   </sheetPr>
   <dimension ref="A1:BC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates for better codecov
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E55035-87AD-4817-805C-93CB3C553B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE300623-3460-4B62-B733-45D44687918A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1740" windowWidth="29040" windowHeight="17640" tabRatio="953" firstSheet="83" activeTab="91" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="953" firstSheet="87" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="290">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1006,15 +1006,6 @@
   </si>
   <si>
     <t>pipeline_expansion_lead_time</t>
-  </si>
-  <si>
-    <t>N10</t>
-  </si>
-  <si>
-    <t>N12</t>
-  </si>
-  <si>
-    <t>N11</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1667,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1999,11 +1990,6 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2222,8 +2208,8 @@
       <sheetName val="PipelineExpansionLeadTime_Capac"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
@@ -2306,88 +2292,88 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64" refreshError="1"/>
-      <sheetData sheetId="65" refreshError="1"/>
-      <sheetData sheetId="66" refreshError="1"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
-      <sheetData sheetId="69" refreshError="1"/>
-      <sheetData sheetId="70" refreshError="1"/>
-      <sheetData sheetId="71" refreshError="1"/>
-      <sheetData sheetId="72" refreshError="1"/>
-      <sheetData sheetId="73" refreshError="1"/>
-      <sheetData sheetId="74" refreshError="1"/>
-      <sheetData sheetId="75" refreshError="1"/>
-      <sheetData sheetId="76" refreshError="1"/>
-      <sheetData sheetId="77" refreshError="1"/>
-      <sheetData sheetId="78" refreshError="1"/>
-      <sheetData sheetId="79" refreshError="1"/>
-      <sheetData sheetId="80" refreshError="1"/>
-      <sheetData sheetId="81" refreshError="1"/>
-      <sheetData sheetId="82" refreshError="1"/>
-      <sheetData sheetId="83" refreshError="1"/>
-      <sheetData sheetId="84" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3433,7 +3419,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4034,7 +4020,7 @@
   <dimension ref="C3:M36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20516,7 +20502,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23602,7 +23588,7 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
@@ -23610,7 +23596,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period", [1]Units!$A$2:$B$11, 2, FALSE),"s]")</f>
         <v>Table of Treatment Expansion Lead Time [weeks]</v>
@@ -23621,7 +23607,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>169</v>
       </c>
@@ -23641,7 +23627,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
@@ -23661,7 +23647,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
         <v>120</v>
       </c>
@@ -23681,7 +23667,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>119</v>
       </c>
@@ -23701,7 +23687,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="70" t="s">
         <v>120</v>
       </c>
@@ -23720,12 +23706,8 @@
       <c r="F6" s="126">
         <v>72</v>
       </c>
-      <c r="J6" s="136"/>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>119</v>
       </c>
@@ -23744,12 +23726,9 @@
       <c r="F7" s="35">
         <v>72</v>
       </c>
-      <c r="J7" s="136"/>
-      <c r="K7" s="137"/>
-      <c r="L7" s="136"/>
-      <c r="M7" s="136"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="70" t="s">
         <v>120</v>
       </c>
@@ -23768,12 +23747,9 @@
       <c r="F8" s="126">
         <v>72</v>
       </c>
-      <c r="J8" s="136"/>
-      <c r="K8" s="137"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="136"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>119</v>
       </c>
@@ -23792,12 +23768,9 @@
       <c r="F9" s="35">
         <v>72</v>
       </c>
-      <c r="J9" s="136"/>
-      <c r="K9" s="137"/>
-      <c r="L9" s="136"/>
-      <c r="M9" s="136"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="70" t="s">
         <v>120</v>
       </c>
@@ -23816,12 +23789,9 @@
       <c r="F10" s="126">
         <v>72</v>
       </c>
-      <c r="J10" s="136"/>
-      <c r="K10" s="137"/>
-      <c r="L10" s="136"/>
-      <c r="M10" s="136"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>119</v>
       </c>
@@ -23840,12 +23810,9 @@
       <c r="F11" s="35">
         <v>72</v>
       </c>
-      <c r="J11" s="136"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="136"/>
-      <c r="M11" s="136"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>120</v>
       </c>
@@ -23864,28 +23831,6 @@
       <c r="F12" s="37">
         <v>72</v>
       </c>
-      <c r="J12" s="136"/>
-      <c r="K12" s="136"/>
-      <c r="L12" s="136"/>
-      <c r="M12" s="136"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J13" s="136"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="136"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J14" s="136"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="136"/>
-      <c r="M14" s="136"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J15" s="136"/>
-      <c r="K15" s="136"/>
-      <c r="L15" s="136"/>
-      <c r="M15" s="136"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23928,7 +23873,7 @@
       <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="138">
+      <c r="B3" s="34">
         <v>0</v>
       </c>
       <c r="C3" s="35">
@@ -23958,7 +23903,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
@@ -23993,13 +23938,13 @@
       <c r="A3" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="138">
-        <v>0</v>
-      </c>
-      <c r="C3" s="138">
+      <c r="B3" s="34">
+        <v>0</v>
+      </c>
+      <c r="C3" s="34">
         <v>88</v>
       </c>
-      <c r="D3" s="138">
+      <c r="D3" s="34">
         <v>89</v>
       </c>
       <c r="E3" s="35">
@@ -24010,13 +23955,13 @@
       <c r="A4" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="B4" s="138">
-        <v>0</v>
-      </c>
-      <c r="C4" s="138">
+      <c r="B4" s="34">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34">
         <v>88</v>
       </c>
-      <c r="D4" s="138">
+      <c r="D4" s="34">
         <v>89</v>
       </c>
       <c r="E4" s="35">
@@ -24095,8 +24040,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24129,10 +24074,10 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>290</v>
+        <v>125</v>
       </c>
       <c r="B3" s="133" t="s">
-        <v>291</v>
+        <v>126</v>
       </c>
       <c r="C3" s="134">
         <v>0</v>
@@ -24146,10 +24091,10 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>291</v>
+        <v>126</v>
       </c>
       <c r="B4" s="133" t="s">
-        <v>290</v>
+        <v>127</v>
       </c>
       <c r="C4" s="134">
         <v>0</v>
@@ -24163,10 +24108,10 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B5" s="133" t="s">
-        <v>292</v>
+        <v>129</v>
       </c>
       <c r="C5" s="134">
         <v>0</v>
@@ -24180,10 +24125,10 @@
     </row>
     <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>292</v>
+        <v>127</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C6" s="128">
         <v>0</v>

</xml_diff>

<commit_message>
update pipeline distance values
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B002C-3CAB-4363-AE0B-20D5CE9BEE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2027B2-087A-4D1C-8929-A3E7239494D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="953" firstSheet="67" activeTab="74" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2389,7 +2389,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21011,10 +21011,10 @@
   </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21844,10 +21844,10 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="77"/>
       <c r="R18" s="7">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S18" s="7">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T18" s="77"/>
       <c r="U18" s="29"/>
@@ -22032,10 +22032,10 @@
         <v>2</v>
       </c>
       <c r="R22" s="7">
-        <v>50</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="S22" s="7">
-        <v>50</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="T22" s="77">
         <v>2</v>
@@ -23245,7 +23245,7 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Hydraulics Post_Process Infeasibility (#273)
* update pipeline distance values

* update obj value in toy case test
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B002C-3CAB-4363-AE0B-20D5CE9BEE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2027B2-087A-4D1C-8929-A3E7239494D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="953" firstSheet="67" activeTab="74" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2389,7 +2389,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21011,10 +21011,10 @@
   </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21844,10 +21844,10 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="77"/>
       <c r="R18" s="7">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="S18" s="7">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="T18" s="77"/>
       <c r="U18" s="29"/>
@@ -22032,10 +22032,10 @@
         <v>2</v>
       </c>
       <c r="R22" s="7">
-        <v>50</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="S22" s="7">
-        <v>50</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="T22" s="77">
         <v>2</v>
@@ -23245,7 +23245,7 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Index disposal capacity increments by individual wells
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48E7CA4-6BA5-4674-8BDA-B75E8523C0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E30C186-FA0E-4A41-B4B2-36644D841BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="291">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -841,9 +841,6 @@
   </si>
   <si>
     <t>PipelineDiameters</t>
-  </si>
-  <si>
-    <t>InjectionCapacities</t>
   </si>
   <si>
     <t>StorageCapacities</t>
@@ -1023,7 +1020,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,14 +1086,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1119,12 +1110,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE4D6"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1673,7 +1658,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1914,12 +1899,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="3" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3080,17 +3059,17 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3130,12 +3109,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -3143,7 +3122,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -4458,17 +4437,17 @@
         <v>117</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="105"/>
       <c r="C3" s="7"/>
       <c r="D3" s="29"/>
     </row>
@@ -4476,7 +4455,7 @@
       <c r="A4" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="7"/>
       <c r="D4" s="29"/>
     </row>
@@ -4484,7 +4463,7 @@
       <c r="A5" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="7"/>
       <c r="D5" s="29"/>
     </row>
@@ -4492,7 +4471,7 @@
       <c r="A6" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="107"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="7"/>
       <c r="D6" s="29"/>
     </row>
@@ -4500,7 +4479,7 @@
       <c r="A7" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="107"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="7"/>
       <c r="D7" s="29"/>
     </row>
@@ -4508,7 +4487,7 @@
       <c r="A8" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="107"/>
+      <c r="B8" s="105"/>
       <c r="C8" s="7"/>
       <c r="D8" s="29"/>
     </row>
@@ -4516,7 +4495,7 @@
       <c r="A9" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="107"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="7"/>
       <c r="D9" s="29"/>
     </row>
@@ -4524,7 +4503,7 @@
       <c r="A10" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="107"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="7"/>
       <c r="D10" s="29"/>
     </row>
@@ -4532,7 +4511,7 @@
       <c r="A11" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="108"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
     </row>
@@ -4561,7 +4540,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4569,20 +4548,20 @@
         <v>161</v>
       </c>
       <c r="B2" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="25" t="s">
         <v>277</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="109"/>
+      <c r="B3" s="107"/>
       <c r="C3" s="7"/>
       <c r="D3" s="29"/>
     </row>
@@ -4590,7 +4569,7 @@
       <c r="A4" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="109"/>
+      <c r="B4" s="107"/>
       <c r="C4" s="7"/>
       <c r="D4" s="29"/>
     </row>
@@ -4598,7 +4577,7 @@
       <c r="A5" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="109"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="7"/>
       <c r="D5" s="29"/>
     </row>
@@ -4606,7 +4585,7 @@
       <c r="A6" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="109"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="7"/>
       <c r="D6" s="29"/>
     </row>
@@ -4614,7 +4593,7 @@
       <c r="A7" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="109"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="7"/>
       <c r="D7" s="29"/>
     </row>
@@ -4622,7 +4601,7 @@
       <c r="A8" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="109"/>
+      <c r="B8" s="107"/>
       <c r="C8" s="7"/>
       <c r="D8" s="29"/>
     </row>
@@ -4630,7 +4609,7 @@
       <c r="A9" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="109"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="7"/>
       <c r="D9" s="29"/>
     </row>
@@ -4638,7 +4617,7 @@
       <c r="A10" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="109"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="7"/>
       <c r="D10" s="29"/>
     </row>
@@ -4646,7 +4625,7 @@
       <c r="A11" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="110"/>
+      <c r="B11" s="108"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
     </row>
@@ -4726,7 +4705,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -4740,7 +4719,7 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -4777,7 +4756,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4785,13 +4764,13 @@
         <v>171</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="25" t="s">
         <v>277</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4800,11 +4779,11 @@
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
-      <c r="D3" s="127"/>
+      <c r="D3" s="125"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
@@ -4812,14 +4791,14 @@
       <c r="C4" s="7">
         <v>1</v>
       </c>
-      <c r="D4" s="127"/>
+      <c r="D4" s="125"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
+        <v>274</v>
+      </c>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
       <c r="D5" s="9">
         <v>1</v>
       </c>
@@ -5096,7 +5075,7 @@
         <v>73</v>
       </c>
       <c r="AZ8" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BA8" s="30" t="s">
         <v>76</v>
@@ -5104,22 +5083,22 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>259</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="D9" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="D9" s="56" t="s">
-        <v>261</v>
-      </c>
       <c r="E9" s="59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F9" s="52" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H9" s="56"/>
       <c r="I9" s="52"/>
@@ -5144,7 +5123,7 @@
         <v>74</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="BA9" s="1" t="s">
         <v>74</v>
@@ -5152,13 +5131,13 @@
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>84</v>
       </c>
       <c r="D10" s="56" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="52"/>
@@ -5186,7 +5165,7 @@
         <v>78</v>
       </c>
       <c r="AZ10" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BA10" s="1" t="s">
         <v>78</v>
@@ -5287,7 +5266,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5336,7 +5315,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5347,10 +5326,10 @@
         <v>117</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5372,8 +5351,8 @@
       <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="128"/>
-      <c r="D4" s="129"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="127"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5442,7 +5421,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -5530,7 +5509,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5538,20 +5517,20 @@
         <v>169</v>
       </c>
       <c r="B2" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="25" t="s">
         <v>277</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="107">
+      <c r="B3" s="105">
         <v>1</v>
       </c>
       <c r="C3" s="7">
@@ -5565,7 +5544,7 @@
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="108"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
     </row>
@@ -5592,7 +5571,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -6004,17 +5983,17 @@
         <v>117</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="108"/>
+      <c r="B3" s="106"/>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
     </row>
@@ -6044,7 +6023,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6055,17 +6034,17 @@
         <v>117</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="105"/>
       <c r="C3" s="7">
         <v>1</v>
       </c>
@@ -6077,7 +6056,7 @@
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="108">
+      <c r="B4" s="106">
         <v>1</v>
       </c>
       <c r="C4" s="8"/>
@@ -6107,7 +6086,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6115,20 +6094,20 @@
         <v>169</v>
       </c>
       <c r="B2" s="73" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="25" t="s">
         <v>277</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="107">
+      <c r="B3" s="105">
         <v>1</v>
       </c>
       <c r="C3" s="7">
@@ -6142,7 +6121,7 @@
       <c r="A4" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="108"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
     </row>
@@ -6170,7 +6149,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6178,13 +6157,13 @@
         <v>171</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="25" t="s">
         <v>277</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6197,7 +6176,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
@@ -6209,7 +6188,7 @@
     </row>
     <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -6240,7 +6219,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -6274,223 +6253,223 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="109" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="100" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="104">
+      <c r="B3" s="102">
         <v>650</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="104">
+      <c r="B4" s="102">
         <v>550</v>
       </c>
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="101" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="104">
+      <c r="B5" s="102">
         <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="122">
+      <c r="B6" s="120">
         <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="121" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="124">
+      <c r="B7" s="122">
         <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="104">
+      <c r="B8" s="102">
         <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="122">
+      <c r="B9" s="120">
         <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="104">
+      <c r="B10" s="102">
         <v>650</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="119" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="122">
+      <c r="B11" s="120">
         <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="104">
+      <c r="B12" s="102">
         <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="101" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="102">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="119" t="s">
         <v>274</v>
       </c>
-      <c r="B13" s="104">
+      <c r="B14" s="120">
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="121" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="102">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="119" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="120">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="101" t="s">
         <v>275</v>
       </c>
-      <c r="B14" s="122">
+      <c r="B17" s="102">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="103" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="104">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="101" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" s="102">
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="121" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="122">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="103" t="s">
-        <v>276</v>
-      </c>
-      <c r="B17" s="104">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="119" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="120">
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="103" t="s">
-        <v>277</v>
-      </c>
-      <c r="B18" s="104">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="121" t="s">
-        <v>278</v>
-      </c>
-      <c r="B19" s="122">
-        <v>500</v>
-      </c>
-    </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="103" t="s">
+      <c r="A20" s="101" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="104">
+      <c r="B20" s="102">
         <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="103" t="s">
+      <c r="A21" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="104">
+      <c r="B21" s="102">
         <v>600</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="101" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="104">
+      <c r="B22" s="102">
         <v>600</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="103" t="s">
+      <c r="A23" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="B23" s="104">
+      <c r="B23" s="102">
         <v>600</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="103" t="s">
+      <c r="A24" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="104">
+      <c r="B24" s="102">
         <v>550</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="104">
+      <c r="B25" s="102">
         <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="103" t="s">
+      <c r="A26" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="104">
+      <c r="B26" s="102">
         <v>550</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="103" t="s">
+      <c r="A27" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="B27" s="104">
+      <c r="B27" s="102">
         <v>550</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="112" t="s">
+      <c r="A28" s="110" t="s">
         <v>133</v>
       </c>
-      <c r="B28" s="113">
+      <c r="B28" s="111">
         <v>500</v>
       </c>
     </row>
@@ -8428,16 +8407,16 @@
   <sheetData>
     <row r="1" spans="1:55" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="Q1" s="1">
         <v>0.01</v>
@@ -9097,160 +9076,160 @@
       <c r="A6" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="125">
+      <c r="B6" s="123">
         <v>20</v>
       </c>
-      <c r="C6" s="125">
+      <c r="C6" s="123">
         <v>19.724654089867183</v>
       </c>
-      <c r="D6" s="125">
+      <c r="D6" s="123">
         <v>19.565347714583421</v>
       </c>
-      <c r="E6" s="125">
+      <c r="E6" s="123">
         <v>19.45309894824571</v>
       </c>
-      <c r="F6" s="125">
+      <c r="F6" s="123">
         <v>19.366475714512596</v>
       </c>
-      <c r="G6" s="125">
+      <c r="G6" s="123">
         <v>19.29598579090657</v>
       </c>
-      <c r="H6" s="125">
+      <c r="H6" s="123">
         <v>19.236587614095988</v>
       </c>
-      <c r="I6" s="125">
+      <c r="I6" s="123">
         <v>19.185282386505289</v>
       </c>
-      <c r="J6" s="125">
+      <c r="J6" s="123">
         <v>19.14014155962774</v>
       </c>
-      <c r="K6" s="125">
+      <c r="K6" s="123">
         <v>19.099851720428717</v>
       </c>
-      <c r="L6" s="125">
+      <c r="L6" s="123">
         <v>19.063478193082773</v>
       </c>
-      <c r="M6" s="125">
+      <c r="M6" s="123">
         <v>19.030332252431219</v>
       </c>
-      <c r="N6" s="125">
+      <c r="N6" s="123">
         <v>18.999891837835946</v>
       </c>
-      <c r="O6" s="125">
+      <c r="O6" s="123">
         <v>18.971751827873344</v>
       </c>
-      <c r="P6" s="125">
+      <c r="P6" s="123">
         <v>18.945591568023726</v>
       </c>
-      <c r="Q6" s="125">
+      <c r="Q6" s="123">
         <v>18.92115293451192</v>
       </c>
-      <c r="R6" s="125">
+      <c r="R6" s="123">
         <v>18.898225082424748</v>
       </c>
-      <c r="S6" s="125">
+      <c r="S6" s="123">
         <v>18.876633574737408</v>
       </c>
-      <c r="T6" s="125">
+      <c r="T6" s="123">
         <v>18.856232464552253</v>
       </c>
-      <c r="U6" s="125">
+      <c r="U6" s="123">
         <v>18.836898417660557</v>
       </c>
-      <c r="V6" s="125">
+      <c r="V6" s="123">
         <v>18.818526275591836</v>
       </c>
-      <c r="W6" s="125">
+      <c r="W6" s="123">
         <v>18.8010256554142</v>
       </c>
-      <c r="X6" s="125">
+      <c r="X6" s="123">
         <v>18.784318308654296</v>
       </c>
-      <c r="Y6" s="125">
+      <c r="Y6" s="123">
         <v>18.768336044722442</v>
       </c>
-      <c r="Z6" s="125">
+      <c r="Z6" s="123">
         <v>18.75301908004031</v>
       </c>
-      <c r="AA6" s="125">
+      <c r="AA6" s="123">
         <v>18.738314712310245</v>
       </c>
-      <c r="AB6" s="125">
+      <c r="AB6" s="123">
         <v>18.724176246023287</v>
       </c>
-      <c r="AC6" s="125">
+      <c r="AC6" s="123">
         <v>18.710562114180359</v>
       </c>
-      <c r="AD6" s="125">
+      <c r="AD6" s="123">
         <v>18.697435154762537</v>
       </c>
-      <c r="AE6" s="125">
+      <c r="AE6" s="123">
         <v>18.684762010358615</v>
       </c>
-      <c r="AF6" s="125">
+      <c r="AF6" s="123">
         <v>18.672512626632653</v>
       </c>
-      <c r="AG6" s="125">
+      <c r="AG6" s="123">
         <v>18.660659830736151</v>
       </c>
-      <c r="AH6" s="125">
+      <c r="AH6" s="123">
         <v>18.649178974852152</v>
       </c>
-      <c r="AI6" s="125">
+      <c r="AI6" s="123">
         <v>18.638047633163993</v>
       </c>
-      <c r="AJ6" s="125">
+      <c r="AJ6" s="123">
         <v>18.627245342924191</v>
       </c>
-      <c r="AK6" s="125">
+      <c r="AK6" s="123">
         <v>18.616753382143422</v>
       </c>
-      <c r="AL6" s="125">
+      <c r="AL6" s="123">
         <v>18.606554577858702</v>
       </c>
-      <c r="AM6" s="125">
+      <c r="AM6" s="123">
         <v>18.59663314007085</v>
       </c>
-      <c r="AN6" s="125">
+      <c r="AN6" s="123">
         <v>18.586974517336788</v>
       </c>
-      <c r="AO6" s="125">
+      <c r="AO6" s="123">
         <v>18.577565270716047</v>
       </c>
-      <c r="AP6" s="125">
+      <c r="AP6" s="123">
         <v>18.568392963342752</v>
       </c>
-      <c r="AQ6" s="125">
+      <c r="AQ6" s="123">
         <v>18.559446063356276</v>
       </c>
-      <c r="AR6" s="125">
+      <c r="AR6" s="123">
         <v>18.550713858298163</v>
       </c>
-      <c r="AS6" s="125">
+      <c r="AS6" s="123">
         <v>18.54218637938818</v>
       </c>
-      <c r="AT6" s="125">
+      <c r="AT6" s="123">
         <v>18.533854334343193</v>
       </c>
-      <c r="AU6" s="125">
+      <c r="AU6" s="123">
         <v>18.525709047608249</v>
       </c>
-      <c r="AV6" s="125">
+      <c r="AV6" s="123">
         <v>18.517742407040306</v>
       </c>
-      <c r="AW6" s="125">
+      <c r="AW6" s="123">
         <v>18.509946816226808</v>
       </c>
-      <c r="AX6" s="125">
+      <c r="AX6" s="123">
         <v>18.502315151739563</v>
       </c>
-      <c r="AY6" s="125">
+      <c r="AY6" s="123">
         <v>18.494840724723719</v>
       </c>
-      <c r="AZ6" s="125">
+      <c r="AZ6" s="123">
         <v>18.48751724630511</v>
       </c>
-      <c r="BA6" s="126">
+      <c r="BA6" s="124">
         <v>18.480338796369434</v>
       </c>
       <c r="BB6" s="83"/>
@@ -10174,19 +10153,19 @@
         <v>117</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q2" s="80" t="s">
         <v>274</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="R2" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="80" t="s">
         <v>277</v>
-      </c>
-      <c r="T2" s="80" t="s">
-        <v>278</v>
       </c>
       <c r="U2" s="25" t="s">
         <v>109</v>
@@ -10235,7 +10214,7 @@
       <c r="N3" s="77">
         <v>0</v>
       </c>
-      <c r="O3" s="107">
+      <c r="O3" s="105">
         <v>0</v>
       </c>
       <c r="P3" s="7"/>
@@ -10290,7 +10269,7 @@
       <c r="N4" s="77">
         <v>0</v>
       </c>
-      <c r="O4" s="107">
+      <c r="O4" s="105">
         <v>0</v>
       </c>
       <c r="P4" s="7"/>
@@ -10345,7 +10324,7 @@
       <c r="N5" s="77">
         <v>0</v>
       </c>
-      <c r="O5" s="107">
+      <c r="O5" s="105">
         <v>0</v>
       </c>
       <c r="P5" s="7"/>
@@ -10400,7 +10379,7 @@
       <c r="N6" s="79">
         <v>0</v>
       </c>
-      <c r="O6" s="115">
+      <c r="O6" s="113">
         <v>0</v>
       </c>
       <c r="P6" s="78"/>
@@ -10455,7 +10434,7 @@
       <c r="N7" s="79">
         <v>0</v>
       </c>
-      <c r="O7" s="115">
+      <c r="O7" s="113">
         <v>0</v>
       </c>
       <c r="P7" s="78"/>
@@ -10510,7 +10489,7 @@
       <c r="N8" s="77">
         <v>0</v>
       </c>
-      <c r="O8" s="107">
+      <c r="O8" s="105">
         <v>0</v>
       </c>
       <c r="P8" s="7"/>
@@ -10563,7 +10542,7 @@
       <c r="N9" s="77">
         <v>0</v>
       </c>
-      <c r="O9" s="107">
+      <c r="O9" s="105">
         <v>0</v>
       </c>
       <c r="P9" s="7"/>
@@ -10616,7 +10595,7 @@
       <c r="N10" s="77">
         <v>0</v>
       </c>
-      <c r="O10" s="107">
+      <c r="O10" s="105">
         <v>0</v>
       </c>
       <c r="P10" s="7"/>
@@ -10669,7 +10648,7 @@
       <c r="N11" s="77">
         <v>0</v>
       </c>
-      <c r="O11" s="107">
+      <c r="O11" s="105">
         <v>0</v>
       </c>
       <c r="P11" s="7"/>
@@ -10722,7 +10701,7 @@
       <c r="N12" s="77">
         <v>0</v>
       </c>
-      <c r="O12" s="107">
+      <c r="O12" s="105">
         <v>0</v>
       </c>
       <c r="P12" s="7"/>
@@ -10775,7 +10754,7 @@
       <c r="N13" s="77">
         <v>0</v>
       </c>
-      <c r="O13" s="107">
+      <c r="O13" s="105">
         <v>0</v>
       </c>
       <c r="P13" s="7"/>
@@ -10828,7 +10807,7 @@
       <c r="N14" s="77">
         <v>0</v>
       </c>
-      <c r="O14" s="107">
+      <c r="O14" s="105">
         <v>0</v>
       </c>
       <c r="P14" s="7"/>
@@ -10879,7 +10858,7 @@
       <c r="N15" s="77">
         <v>0</v>
       </c>
-      <c r="O15" s="107">
+      <c r="O15" s="105">
         <v>0</v>
       </c>
       <c r="P15" s="7"/>
@@ -10934,7 +10913,7 @@
       <c r="N16" s="79">
         <v>0</v>
       </c>
-      <c r="O16" s="115">
+      <c r="O16" s="113">
         <v>0</v>
       </c>
       <c r="P16" s="78"/>
@@ -10989,7 +10968,7 @@
       <c r="N17" s="77">
         <v>0</v>
       </c>
-      <c r="O17" s="107">
+      <c r="O17" s="105">
         <v>0</v>
       </c>
       <c r="P17" s="7"/>
@@ -11003,7 +10982,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -11018,7 +10997,7 @@
       <c r="L18" s="77"/>
       <c r="M18" s="7"/>
       <c r="N18" s="77"/>
-      <c r="O18" s="107"/>
+      <c r="O18" s="105"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="77"/>
       <c r="R18" s="7"/>
@@ -11028,7 +11007,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
@@ -11043,7 +11022,7 @@
       <c r="L19" s="79"/>
       <c r="M19" s="78"/>
       <c r="N19" s="79"/>
-      <c r="O19" s="115"/>
+      <c r="O19" s="113"/>
       <c r="P19" s="78"/>
       <c r="Q19" s="79"/>
       <c r="R19" s="78"/>
@@ -11094,7 +11073,7 @@
       <c r="N20" s="77">
         <v>0</v>
       </c>
-      <c r="O20" s="107">
+      <c r="O20" s="105">
         <v>0</v>
       </c>
       <c r="P20" s="7"/>
@@ -11149,7 +11128,7 @@
       <c r="N21" s="79">
         <v>0</v>
       </c>
-      <c r="O21" s="115">
+      <c r="O21" s="113">
         <v>0</v>
       </c>
       <c r="P21" s="78"/>
@@ -11204,7 +11183,7 @@
       <c r="N22" s="77">
         <v>0</v>
       </c>
-      <c r="O22" s="107">
+      <c r="O22" s="105">
         <v>0</v>
       </c>
       <c r="P22" s="7"/>
@@ -11259,7 +11238,7 @@
       <c r="N23" s="82">
         <v>0</v>
       </c>
-      <c r="O23" s="108">
+      <c r="O23" s="106">
         <v>71429</v>
       </c>
       <c r="P23" s="8"/>
@@ -11302,7 +11281,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
@@ -11352,58 +11331,58 @@
         <v>117</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q2" s="80" t="s">
         <v>274</v>
-      </c>
-      <c r="Q2" s="80" t="s">
-        <v>275</v>
       </c>
       <c r="R2" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105"/>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="105"/>
-      <c r="Z2" s="105"/>
-      <c r="AA2" s="105"/>
-      <c r="AB2" s="105"/>
-      <c r="AC2" s="105"/>
-      <c r="AD2" s="105"/>
-      <c r="AE2" s="105"/>
-      <c r="AF2" s="105"/>
-      <c r="AG2" s="105"/>
-      <c r="AH2" s="105"/>
-      <c r="AI2" s="105"/>
-      <c r="AJ2" s="105"/>
-      <c r="AK2" s="105"/>
-      <c r="AL2" s="105"/>
-      <c r="AM2" s="105"/>
-      <c r="AN2" s="105"/>
-      <c r="AO2" s="105"/>
-      <c r="AP2" s="105"/>
-      <c r="AQ2" s="105"/>
-      <c r="AR2" s="105"/>
-      <c r="AS2" s="105"/>
-      <c r="AT2" s="105"/>
-      <c r="AU2" s="105"/>
-      <c r="AV2" s="105"/>
-      <c r="AW2" s="105"/>
-      <c r="AX2" s="105"/>
-      <c r="AY2" s="105"/>
-      <c r="AZ2" s="105"/>
-      <c r="BA2" s="105"/>
-      <c r="BB2" s="105"/>
-      <c r="BC2" s="105"/>
-      <c r="BD2" s="105"/>
-      <c r="BE2" s="105"/>
-      <c r="BF2" s="105"/>
-      <c r="BG2" s="105"/>
-      <c r="BH2" s="105"/>
-      <c r="BI2" s="105"/>
-      <c r="BJ2" s="105"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="103"/>
+      <c r="AB2" s="103"/>
+      <c r="AC2" s="103"/>
+      <c r="AD2" s="103"/>
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="103"/>
+      <c r="AG2" s="103"/>
+      <c r="AH2" s="103"/>
+      <c r="AI2" s="103"/>
+      <c r="AJ2" s="103"/>
+      <c r="AK2" s="103"/>
+      <c r="AL2" s="103"/>
+      <c r="AM2" s="103"/>
+      <c r="AN2" s="103"/>
+      <c r="AO2" s="103"/>
+      <c r="AP2" s="103"/>
+      <c r="AQ2" s="103"/>
+      <c r="AR2" s="103"/>
+      <c r="AS2" s="103"/>
+      <c r="AT2" s="103"/>
+      <c r="AU2" s="103"/>
+      <c r="AV2" s="103"/>
+      <c r="AW2" s="103"/>
+      <c r="AX2" s="103"/>
+      <c r="AY2" s="103"/>
+      <c r="AZ2" s="103"/>
+      <c r="BA2" s="103"/>
+      <c r="BB2" s="103"/>
+      <c r="BC2" s="103"/>
+      <c r="BD2" s="103"/>
+      <c r="BE2" s="103"/>
+      <c r="BF2" s="103"/>
+      <c r="BG2" s="103"/>
+      <c r="BH2" s="103"/>
+      <c r="BI2" s="103"/>
+      <c r="BJ2" s="103"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -11424,7 +11403,7 @@
       <c r="L3" s="77"/>
       <c r="M3" s="7"/>
       <c r="N3" s="77"/>
-      <c r="O3" s="107"/>
+      <c r="O3" s="105"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="77"/>
       <c r="R3" s="29"/>
@@ -11492,7 +11471,7 @@
       <c r="L4" s="77"/>
       <c r="M4" s="7"/>
       <c r="N4" s="77"/>
-      <c r="O4" s="107"/>
+      <c r="O4" s="105"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="77"/>
       <c r="R4" s="29"/>
@@ -11560,7 +11539,7 @@
       <c r="L5" s="77"/>
       <c r="M5" s="7"/>
       <c r="N5" s="77"/>
-      <c r="O5" s="107"/>
+      <c r="O5" s="105"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="77"/>
       <c r="R5" s="29"/>
@@ -11626,7 +11605,7 @@
       <c r="L6" s="79"/>
       <c r="M6" s="78"/>
       <c r="N6" s="79"/>
-      <c r="O6" s="115"/>
+      <c r="O6" s="113"/>
       <c r="P6" s="78"/>
       <c r="Q6" s="79"/>
       <c r="R6" s="81"/>
@@ -11694,7 +11673,7 @@
       <c r="L7" s="79"/>
       <c r="M7" s="78"/>
       <c r="N7" s="79"/>
-      <c r="O7" s="115"/>
+      <c r="O7" s="113"/>
       <c r="P7" s="78"/>
       <c r="Q7" s="79"/>
       <c r="R7" s="81"/>
@@ -11764,7 +11743,7 @@
       <c r="L8" s="77"/>
       <c r="M8" s="7"/>
       <c r="N8" s="77"/>
-      <c r="O8" s="107"/>
+      <c r="O8" s="105"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="77"/>
       <c r="R8" s="29"/>
@@ -11834,7 +11813,7 @@
       <c r="L9" s="77"/>
       <c r="M9" s="7"/>
       <c r="N9" s="77"/>
-      <c r="O9" s="107"/>
+      <c r="O9" s="105"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="77"/>
       <c r="R9" s="29"/>
@@ -11902,7 +11881,7 @@
       <c r="L10" s="77"/>
       <c r="M10" s="7"/>
       <c r="N10" s="77"/>
-      <c r="O10" s="107"/>
+      <c r="O10" s="105"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="77"/>
       <c r="R10" s="29"/>
@@ -11972,7 +11951,7 @@
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="77"/>
-      <c r="O11" s="107"/>
+      <c r="O11" s="105"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="77"/>
       <c r="R11" s="29"/>
@@ -12040,7 +12019,7 @@
       <c r="L12" s="77"/>
       <c r="M12" s="7"/>
       <c r="N12" s="77"/>
-      <c r="O12" s="107"/>
+      <c r="O12" s="105"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="77"/>
       <c r="R12" s="29"/>
@@ -12108,7 +12087,7 @@
       <c r="L13" s="77"/>
       <c r="M13" s="7"/>
       <c r="N13" s="77"/>
-      <c r="O13" s="107"/>
+      <c r="O13" s="105"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="77"/>
       <c r="R13" s="29"/>
@@ -12176,7 +12155,7 @@
       <c r="L14" s="77"/>
       <c r="M14" s="7"/>
       <c r="N14" s="77"/>
-      <c r="O14" s="107"/>
+      <c r="O14" s="105"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="77"/>
       <c r="R14" s="29"/>
@@ -12242,7 +12221,7 @@
       <c r="L15" s="77"/>
       <c r="M15" s="7"/>
       <c r="N15" s="77"/>
-      <c r="O15" s="107"/>
+      <c r="O15" s="105"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="77"/>
       <c r="R15" s="29"/>
@@ -12308,7 +12287,7 @@
       <c r="L16" s="79"/>
       <c r="M16" s="78"/>
       <c r="N16" s="79"/>
-      <c r="O16" s="115"/>
+      <c r="O16" s="113"/>
       <c r="P16" s="78"/>
       <c r="Q16" s="79"/>
       <c r="R16" s="81"/>
@@ -12374,7 +12353,7 @@
       <c r="L17" s="77"/>
       <c r="M17" s="7"/>
       <c r="N17" s="77"/>
-      <c r="O17" s="107"/>
+      <c r="O17" s="105"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="77"/>
       <c r="R17" s="29"/>
@@ -12425,7 +12404,7 @@
     </row>
     <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -12440,7 +12419,7 @@
       <c r="L18" s="77"/>
       <c r="M18" s="7"/>
       <c r="N18" s="77"/>
-      <c r="O18" s="107"/>
+      <c r="O18" s="105"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="77"/>
       <c r="R18" s="29"/>
@@ -12491,7 +12470,7 @@
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
@@ -12506,7 +12485,7 @@
       <c r="L19" s="79"/>
       <c r="M19" s="78"/>
       <c r="N19" s="79"/>
-      <c r="O19" s="115"/>
+      <c r="O19" s="113"/>
       <c r="P19" s="78"/>
       <c r="Q19" s="79"/>
       <c r="R19" s="81"/>
@@ -12572,7 +12551,7 @@
       <c r="L20" s="77"/>
       <c r="M20" s="7"/>
       <c r="N20" s="77"/>
-      <c r="O20" s="107"/>
+      <c r="O20" s="105"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="77"/>
       <c r="R20" s="29">
@@ -12640,7 +12619,7 @@
       <c r="L21" s="79"/>
       <c r="M21" s="78"/>
       <c r="N21" s="79"/>
-      <c r="O21" s="115"/>
+      <c r="O21" s="113"/>
       <c r="P21" s="78"/>
       <c r="Q21" s="79"/>
       <c r="R21" s="81">
@@ -12708,7 +12687,7 @@
       <c r="L22" s="77"/>
       <c r="M22" s="7"/>
       <c r="N22" s="77"/>
-      <c r="O22" s="107"/>
+      <c r="O22" s="105"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="77"/>
       <c r="R22" s="29"/>
@@ -12774,7 +12753,7 @@
       <c r="L23" s="82"/>
       <c r="M23" s="8"/>
       <c r="N23" s="82"/>
-      <c r="O23" s="108">
+      <c r="O23" s="106">
         <v>8</v>
       </c>
       <c r="P23" s="8"/>
@@ -12826,7 +12805,7 @@
       <c r="BJ23" s="6"/>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A24" s="106"/>
+      <c r="A24" s="104"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -12890,7 +12869,7 @@
       <c r="BJ24" s="6"/>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A25" s="106"/>
+      <c r="A25" s="104"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -12954,7 +12933,7 @@
       <c r="BJ25" s="6"/>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A26" s="106"/>
+      <c r="A26" s="104"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -13018,7 +12997,7 @@
       <c r="BJ26" s="6"/>
     </row>
     <row r="27" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
+      <c r="A27" s="104"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -13082,7 +13061,7 @@
       <c r="BJ27" s="6"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A28" s="106"/>
+      <c r="A28" s="104"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -13146,7 +13125,7 @@
       <c r="BJ28" s="6"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A29" s="106"/>
+      <c r="A29" s="104"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -13210,7 +13189,7 @@
       <c r="BJ29" s="6"/>
     </row>
     <row r="30" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A30" s="106"/>
+      <c r="A30" s="104"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -13274,7 +13253,7 @@
       <c r="BJ30" s="6"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A31" s="106"/>
+      <c r="A31" s="104"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -13338,7 +13317,7 @@
       <c r="BJ31" s="6"/>
     </row>
     <row r="32" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A32" s="106"/>
+      <c r="A32" s="104"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -13402,7 +13381,7 @@
       <c r="BJ32" s="6"/>
     </row>
     <row r="33" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A33" s="106"/>
+      <c r="A33" s="104"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -13466,7 +13445,7 @@
       <c r="BJ33" s="6"/>
     </row>
     <row r="34" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A34" s="106"/>
+      <c r="A34" s="104"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -13530,7 +13509,7 @@
       <c r="BJ34" s="6"/>
     </row>
     <row r="35" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A35" s="106"/>
+      <c r="A35" s="104"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -13594,7 +13573,7 @@
       <c r="BJ35" s="6"/>
     </row>
     <row r="36" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A36" s="106"/>
+      <c r="A36" s="104"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -13658,7 +13637,7 @@
       <c r="BJ36" s="6"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A37" s="106"/>
+      <c r="A37" s="104"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -13722,7 +13701,7 @@
       <c r="BJ37" s="6"/>
     </row>
     <row r="38" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A38" s="106"/>
+      <c r="A38" s="104"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -13786,7 +13765,7 @@
       <c r="BJ38" s="6"/>
     </row>
     <row r="39" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A39" s="106"/>
+      <c r="A39" s="104"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -13850,7 +13829,7 @@
       <c r="BJ39" s="6"/>
     </row>
     <row r="40" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A40" s="106"/>
+      <c r="A40" s="104"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -13914,7 +13893,7 @@
       <c r="BJ40" s="6"/>
     </row>
     <row r="41" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A41" s="106"/>
+      <c r="A41" s="104"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -13978,7 +13957,7 @@
       <c r="BJ41" s="6"/>
     </row>
     <row r="42" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A42" s="106"/>
+      <c r="A42" s="104"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -14042,7 +14021,7 @@
       <c r="BJ42" s="6"/>
     </row>
     <row r="43" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A43" s="106"/>
+      <c r="A43" s="104"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -14106,7 +14085,7 @@
       <c r="BJ43" s="6"/>
     </row>
     <row r="44" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A44" s="106"/>
+      <c r="A44" s="104"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -14170,7 +14149,7 @@
       <c r="BJ44" s="6"/>
     </row>
     <row r="45" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A45" s="106"/>
+      <c r="A45" s="104"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -14234,7 +14213,7 @@
       <c r="BJ45" s="6"/>
     </row>
     <row r="46" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A46" s="106"/>
+      <c r="A46" s="104"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -14298,7 +14277,7 @@
       <c r="BJ46" s="6"/>
     </row>
     <row r="47" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A47" s="106"/>
+      <c r="A47" s="104"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -14362,7 +14341,7 @@
       <c r="BJ47" s="6"/>
     </row>
     <row r="48" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A48" s="106"/>
+      <c r="A48" s="104"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -14426,7 +14405,7 @@
       <c r="BJ48" s="6"/>
     </row>
     <row r="49" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A49" s="106"/>
+      <c r="A49" s="104"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -14490,7 +14469,7 @@
       <c r="BJ49" s="6"/>
     </row>
     <row r="50" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A50" s="106"/>
+      <c r="A50" s="104"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -14554,7 +14533,7 @@
       <c r="BJ50" s="6"/>
     </row>
     <row r="51" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A51" s="106"/>
+      <c r="A51" s="104"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -14618,7 +14597,7 @@
       <c r="BJ51" s="6"/>
     </row>
     <row r="52" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A52" s="106"/>
+      <c r="A52" s="104"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -14682,7 +14661,7 @@
       <c r="BJ52" s="6"/>
     </row>
     <row r="53" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A53" s="106"/>
+      <c r="A53" s="104"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -14746,7 +14725,7 @@
       <c r="BJ53" s="6"/>
     </row>
     <row r="54" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A54" s="106"/>
+      <c r="A54" s="104"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -14810,7 +14789,7 @@
       <c r="BJ54" s="6"/>
     </row>
     <row r="55" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A55" s="106"/>
+      <c r="A55" s="104"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
@@ -14874,7 +14853,7 @@
       <c r="BJ55" s="6"/>
     </row>
     <row r="56" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A56" s="106"/>
+      <c r="A56" s="104"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -14938,7 +14917,7 @@
       <c r="BJ56" s="6"/>
     </row>
     <row r="57" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A57" s="106"/>
+      <c r="A57" s="104"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -15002,7 +14981,7 @@
       <c r="BJ57" s="6"/>
     </row>
     <row r="58" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A58" s="106"/>
+      <c r="A58" s="104"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -15066,7 +15045,7 @@
       <c r="BJ58" s="6"/>
     </row>
     <row r="59" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A59" s="106"/>
+      <c r="A59" s="104"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
@@ -15130,7 +15109,7 @@
       <c r="BJ59" s="6"/>
     </row>
     <row r="60" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A60" s="106"/>
+      <c r="A60" s="104"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -15194,7 +15173,7 @@
       <c r="BJ60" s="6"/>
     </row>
     <row r="61" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A61" s="106"/>
+      <c r="A61" s="104"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -15258,7 +15237,7 @@
       <c r="BJ61" s="6"/>
     </row>
     <row r="62" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A62" s="106"/>
+      <c r="A62" s="104"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
@@ -15322,7 +15301,7 @@
       <c r="BJ62" s="6"/>
     </row>
     <row r="63" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A63" s="106"/>
+      <c r="A63" s="104"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -15486,7 +15465,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="35">
         <v>0</v>
@@ -15494,7 +15473,7 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="37">
         <v>0</v>
@@ -15540,13 +15519,13 @@
         <v>122</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="25" t="s">
         <v>256</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -15620,7 +15599,7 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>178</v>
@@ -15781,7 +15760,7 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
@@ -15942,7 +15921,7 @@
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="34">
         <v>0</v>
@@ -16103,7 +16082,7 @@
     </row>
     <row r="5" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="36">
         <v>0</v>
@@ -16292,7 +16271,7 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>178</v>
@@ -16453,7 +16432,7 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
@@ -16614,7 +16593,7 @@
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="34">
         <v>12580</v>
@@ -16775,7 +16754,7 @@
     </row>
     <row r="5" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="36">
         <v>51112</v>
@@ -16974,7 +16953,7 @@
         <v>42857.142857142899</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L1" s="1">
         <v>0.7</v>
@@ -18327,7 +18306,7 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -18475,7 +18454,7 @@
         <v>119</v>
       </c>
       <c r="B7" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="29">
         <v>0.5</v>
@@ -18486,7 +18465,7 @@
         <v>120</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="29">
         <v>0.5</v>
@@ -18497,7 +18476,7 @@
         <v>119</v>
       </c>
       <c r="B9" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="29">
         <v>1</v>
@@ -18508,7 +18487,7 @@
         <v>120</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="29">
         <v>1</v>
@@ -18519,7 +18498,7 @@
         <v>119</v>
       </c>
       <c r="B11" s="84" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" s="29">
         <v>0.7</v>
@@ -18530,7 +18509,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="87" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" s="9">
         <v>0.7</v>
@@ -18658,19 +18637,19 @@
         <v>117</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q2" s="80" t="s">
         <v>274</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="R2" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="80" t="s">
         <v>277</v>
-      </c>
-      <c r="T2" s="80" t="s">
-        <v>278</v>
       </c>
       <c r="U2" s="25" t="s">
         <v>109</v>
@@ -18719,7 +18698,7 @@
       <c r="N3" s="77">
         <v>0</v>
       </c>
-      <c r="O3" s="107">
+      <c r="O3" s="105">
         <v>0</v>
       </c>
       <c r="P3" s="7">
@@ -18784,7 +18763,7 @@
       <c r="N4" s="77">
         <v>0</v>
       </c>
-      <c r="O4" s="107">
+      <c r="O4" s="105">
         <v>0</v>
       </c>
       <c r="P4" s="7">
@@ -18849,7 +18828,7 @@
       <c r="N5" s="77">
         <v>0</v>
       </c>
-      <c r="O5" s="107">
+      <c r="O5" s="105">
         <v>0</v>
       </c>
       <c r="P5" s="7">
@@ -18914,7 +18893,7 @@
       <c r="N6" s="79">
         <v>0</v>
       </c>
-      <c r="O6" s="115">
+      <c r="O6" s="113">
         <v>0</v>
       </c>
       <c r="P6" s="78">
@@ -18979,7 +18958,7 @@
       <c r="N7" s="79">
         <v>0</v>
       </c>
-      <c r="O7" s="115">
+      <c r="O7" s="113">
         <v>0</v>
       </c>
       <c r="P7" s="78">
@@ -19044,7 +19023,7 @@
       <c r="N8" s="77">
         <v>0</v>
       </c>
-      <c r="O8" s="107">
+      <c r="O8" s="105">
         <v>0</v>
       </c>
       <c r="P8" s="7">
@@ -19109,7 +19088,7 @@
       <c r="N9" s="77">
         <v>0</v>
       </c>
-      <c r="O9" s="107">
+      <c r="O9" s="105">
         <v>0</v>
       </c>
       <c r="P9" s="7">
@@ -19174,7 +19153,7 @@
       <c r="N10" s="77">
         <v>0</v>
       </c>
-      <c r="O10" s="107">
+      <c r="O10" s="105">
         <v>0</v>
       </c>
       <c r="P10" s="7">
@@ -19239,7 +19218,7 @@
       <c r="N11" s="77">
         <v>0</v>
       </c>
-      <c r="O11" s="107">
+      <c r="O11" s="105">
         <v>0</v>
       </c>
       <c r="P11" s="7">
@@ -19304,7 +19283,7 @@
       <c r="N12" s="77">
         <v>0</v>
       </c>
-      <c r="O12" s="107">
+      <c r="O12" s="105">
         <v>0</v>
       </c>
       <c r="P12" s="7">
@@ -19369,7 +19348,7 @@
       <c r="N13" s="77">
         <v>0</v>
       </c>
-      <c r="O13" s="107">
+      <c r="O13" s="105">
         <v>0</v>
       </c>
       <c r="P13" s="7">
@@ -19434,7 +19413,7 @@
       <c r="N14" s="77">
         <v>0</v>
       </c>
-      <c r="O14" s="107">
+      <c r="O14" s="105">
         <v>0</v>
       </c>
       <c r="P14" s="7">
@@ -19499,7 +19478,7 @@
       <c r="N15" s="77">
         <v>0</v>
       </c>
-      <c r="O15" s="107">
+      <c r="O15" s="105">
         <v>0</v>
       </c>
       <c r="P15" s="7">
@@ -19564,7 +19543,7 @@
       <c r="N16" s="79">
         <v>1E-4</v>
       </c>
-      <c r="O16" s="115">
+      <c r="O16" s="113">
         <v>0</v>
       </c>
       <c r="P16" s="78">
@@ -19629,7 +19608,7 @@
       <c r="N17" s="77">
         <v>0</v>
       </c>
-      <c r="O17" s="107">
+      <c r="O17" s="105">
         <v>0</v>
       </c>
       <c r="P17" s="7">
@@ -19638,13 +19617,13 @@
       <c r="Q17" s="77">
         <v>0</v>
       </c>
-      <c r="R17" s="116">
-        <v>0</v>
-      </c>
-      <c r="S17" s="117">
-        <v>0</v>
-      </c>
-      <c r="T17" s="114">
+      <c r="R17" s="114">
+        <v>0</v>
+      </c>
+      <c r="S17" s="115">
+        <v>0</v>
+      </c>
+      <c r="T17" s="112">
         <v>0</v>
       </c>
       <c r="U17" s="29">
@@ -19653,7 +19632,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B18" s="7">
         <v>0</v>
@@ -19694,7 +19673,7 @@
       <c r="N18" s="77">
         <v>0</v>
       </c>
-      <c r="O18" s="107">
+      <c r="O18" s="105">
         <v>0</v>
       </c>
       <c r="P18" s="7">
@@ -19703,7 +19682,7 @@
       <c r="Q18" s="77">
         <v>0</v>
       </c>
-      <c r="R18" s="107">
+      <c r="R18" s="105">
         <v>1E-4</v>
       </c>
       <c r="S18" s="7">
@@ -19718,7 +19697,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" s="78">
         <v>0</v>
@@ -19759,7 +19738,7 @@
       <c r="N19" s="79">
         <v>0</v>
       </c>
-      <c r="O19" s="115">
+      <c r="O19" s="113">
         <v>0</v>
       </c>
       <c r="P19" s="78">
@@ -19768,7 +19747,7 @@
       <c r="Q19" s="79">
         <v>0</v>
       </c>
-      <c r="R19" s="115">
+      <c r="R19" s="113">
         <v>0</v>
       </c>
       <c r="S19" s="78">
@@ -19824,7 +19803,7 @@
       <c r="N20" s="77">
         <v>0</v>
       </c>
-      <c r="O20" s="107">
+      <c r="O20" s="105">
         <v>0</v>
       </c>
       <c r="P20" s="7">
@@ -19889,7 +19868,7 @@
       <c r="N21" s="79">
         <v>0</v>
       </c>
-      <c r="O21" s="115">
+      <c r="O21" s="113">
         <v>0</v>
       </c>
       <c r="P21" s="78">
@@ -19954,7 +19933,7 @@
       <c r="N22" s="77">
         <v>0</v>
       </c>
-      <c r="O22" s="107">
+      <c r="O22" s="105">
         <v>0</v>
       </c>
       <c r="P22" s="7">
@@ -19966,7 +19945,7 @@
       <c r="R22" s="7">
         <v>1E-4</v>
       </c>
-      <c r="S22" s="117">
+      <c r="S22" s="115">
         <v>1E-4</v>
       </c>
       <c r="T22" s="77">
@@ -20019,7 +19998,7 @@
       <c r="N23" s="82">
         <v>0</v>
       </c>
-      <c r="O23" s="108">
+      <c r="O23" s="106">
         <v>1E-4</v>
       </c>
       <c r="P23" s="8">
@@ -20347,7 +20326,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20425,10 +20404,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20437,49 +20416,60 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Disposal Capacity Expansion Increments [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="101">
+        <v>111</v>
+      </c>
+      <c r="B3" s="34">
+        <v>0</v>
+      </c>
+      <c r="C3" s="34">
         <v>7143</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="101">
+      <c r="D3" s="34">
         <v>14286</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="100">
+      <c r="E3" s="43">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="36">
+        <v>0</v>
+      </c>
+      <c r="C4" s="36">
+        <v>7143</v>
+      </c>
+      <c r="D4" s="36">
+        <v>14286</v>
+      </c>
+      <c r="E4" s="37">
         <v>50000</v>
       </c>
     </row>
@@ -20548,7 +20538,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="34">
         <v>18</v>
@@ -20565,7 +20555,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="36">
         <v>21</v>
@@ -20611,7 +20601,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>46</v>
@@ -20784,7 +20774,7 @@
         <v>119</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="34">
         <v>1000</v>
@@ -20804,7 +20794,7 @@
         <v>120</v>
       </c>
       <c r="B8" s="76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="34">
         <v>1000</v>
@@ -20824,7 +20814,7 @@
         <v>119</v>
       </c>
       <c r="B9" s="76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="34">
         <v>500</v>
@@ -20844,7 +20834,7 @@
         <v>120</v>
       </c>
       <c r="B10" s="76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="34">
         <v>500</v>
@@ -20864,7 +20854,7 @@
         <v>119</v>
       </c>
       <c r="B11" s="76" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" s="34">
         <v>800</v>
@@ -20884,7 +20874,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" s="36">
         <v>800</v>
@@ -20932,7 +20922,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>146</v>
@@ -20983,7 +20973,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" s="34">
         <v>0</v>
@@ -21000,7 +20990,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" s="34">
         <v>0</v>
@@ -21017,7 +21007,7 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" s="36">
         <v>0</v>
@@ -21073,12 +21063,12 @@
         <v>45</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" s="37">
         <v>300000</v>
@@ -21160,19 +21150,19 @@
         <v>117</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q2" s="80" t="s">
         <v>274</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="R2" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="80" t="s">
         <v>277</v>
-      </c>
-      <c r="T2" s="80" t="s">
-        <v>278</v>
       </c>
       <c r="U2" s="25" t="s">
         <v>109</v>
@@ -21186,41 +21176,41 @@
         <v>1.4259999999999999</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J3" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L3" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N3" s="77"/>
-      <c r="O3" s="107" t="s">
-        <v>242</v>
+      <c r="O3" s="105" t="s">
+        <v>241</v>
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="77"/>
@@ -21228,7 +21218,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="77"/>
       <c r="U3" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -21236,44 +21226,44 @@
         <v>90</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="7">
         <v>1.6847000000000001</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J4" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L4" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N4" s="77"/>
-      <c r="O4" s="107" t="s">
-        <v>242</v>
+      <c r="O4" s="105" t="s">
+        <v>241</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="77"/>
@@ -21281,7 +21271,7 @@
       <c r="S4" s="7"/>
       <c r="T4" s="77"/>
       <c r="U4" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -21289,44 +21279,44 @@
         <v>91</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G5" s="7">
         <v>1.2563</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J5" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L5" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N5" s="77"/>
-      <c r="O5" s="107" t="s">
-        <v>242</v>
+      <c r="O5" s="105" t="s">
+        <v>241</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="77"/>
@@ -21334,7 +21324,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="77"/>
       <c r="U5" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -21342,44 +21332,44 @@
         <v>92</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J6" s="79">
         <v>2.5074000000000001</v>
       </c>
       <c r="K6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L6" s="79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M6" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N6" s="79"/>
-      <c r="O6" s="115" t="s">
-        <v>242</v>
+      <c r="O6" s="113" t="s">
+        <v>241</v>
       </c>
       <c r="P6" s="78"/>
       <c r="Q6" s="79"/>
@@ -21387,7 +21377,7 @@
       <c r="S6" s="78"/>
       <c r="T6" s="79"/>
       <c r="U6" s="81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -21395,41 +21385,41 @@
         <v>109</v>
       </c>
       <c r="B7" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D7" s="92"/>
       <c r="E7" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F7" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G7" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H7" s="92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I7" s="92">
         <f>2*F4</f>
         <v>3.3694000000000002</v>
       </c>
       <c r="J7" s="79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K7" s="93" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L7" s="96" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M7" s="92"/>
       <c r="N7" s="95"/>
-      <c r="O7" s="119" t="s">
-        <v>242</v>
+      <c r="O7" s="117" t="s">
+        <v>241</v>
       </c>
       <c r="P7" s="92"/>
       <c r="Q7" s="95"/>
@@ -21437,51 +21427,51 @@
       <c r="S7" s="92"/>
       <c r="T7" s="95"/>
       <c r="U7" s="94" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="120" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" s="120">
+      <c r="B8" s="118" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="118">
         <v>4.0752409775985399</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J8" s="77" t="s">
-        <v>242</v>
-      </c>
-      <c r="K8" s="120">
+        <v>241</v>
+      </c>
+      <c r="K8" s="118">
         <v>4.1717000000000004</v>
       </c>
       <c r="L8" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N8" s="77"/>
-      <c r="O8" s="107"/>
+      <c r="O8" s="105"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="77"/>
       <c r="R8" s="7"/>
@@ -21493,44 +21483,44 @@
       <c r="A9" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="118">
         <v>4.0752409775985399</v>
       </c>
-      <c r="C9" s="120" t="s">
-        <v>242</v>
+      <c r="C9" s="118" t="s">
+        <v>241</v>
       </c>
       <c r="D9" s="7">
         <v>8.2970000000000006</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F9" s="7">
         <v>1.8142</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J9" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L9" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N9" s="77"/>
-      <c r="O9" s="107"/>
+      <c r="O9" s="105"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="77"/>
       <c r="R9" s="7"/>
@@ -21543,43 +21533,43 @@
         <v>127</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C10" s="7">
         <v>8.2970000000000006</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E10" s="7">
         <v>8.3129999999999988</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J10" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L10" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M10" s="7">
         <v>1.4</v>
       </c>
       <c r="N10" s="77"/>
-      <c r="O10" s="107"/>
+      <c r="O10" s="105"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="77"/>
       <c r="R10" s="7"/>
@@ -21592,43 +21582,43 @@
         <v>128</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="7">
         <v>8.3129999999999988</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G11" s="7">
         <v>1.2533000000000001</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J11" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L11" s="77">
         <v>1.3163</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N11" s="77"/>
-      <c r="O11" s="107"/>
+      <c r="O11" s="105"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="77"/>
       <c r="R11" s="7"/>
@@ -21641,43 +21631,43 @@
         <v>129</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" s="120">
+        <v>241</v>
+      </c>
+      <c r="C12" s="118">
         <v>1.8142</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I12" s="7">
         <v>1.4431</v>
       </c>
       <c r="J12" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L12" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N12" s="77"/>
-      <c r="O12" s="107"/>
+      <c r="O12" s="105"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="77"/>
       <c r="R12" s="7"/>
@@ -21690,43 +21680,43 @@
         <v>130</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E13" s="7">
         <v>1.2533000000000001</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H13" s="7">
         <v>1.153</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J13" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L13" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N13" s="77"/>
-      <c r="O13" s="107"/>
+      <c r="O13" s="105"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="77"/>
       <c r="R13" s="7"/>
@@ -21739,25 +21729,25 @@
         <v>131</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G14" s="7">
         <v>1.153</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I14" s="7">
         <v>6.0780000000000003</v>
@@ -21766,16 +21756,16 @@
         <v>2.4449000000000001</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L14" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N14" s="77"/>
-      <c r="O14" s="107"/>
+      <c r="O14" s="105"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="77"/>
       <c r="R14" s="7"/>
@@ -21788,41 +21778,41 @@
         <v>132</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F15" s="7">
         <v>1.4431</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H15" s="7">
         <v>6.0780000000000003</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J15" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L15" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M15" s="7"/>
       <c r="N15" s="77"/>
-      <c r="O15" s="107"/>
+      <c r="O15" s="105"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="77"/>
       <c r="R15" s="7"/>
@@ -21835,45 +21825,45 @@
         <v>133</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H16" s="7">
         <v>2.4449000000000001</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J16" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L16" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N16" s="77">
         <v>2.5</v>
       </c>
-      <c r="O16" s="107"/>
+      <c r="O16" s="105"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="77"/>
       <c r="R16" s="7"/>
@@ -21885,32 +21875,32 @@
       <c r="A17" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="117"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="114"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="114"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="114"/>
-      <c r="O17" s="116"/>
-      <c r="P17" s="117"/>
-      <c r="Q17" s="114"/>
-      <c r="R17" s="117"/>
-      <c r="S17" s="117"/>
-      <c r="T17" s="114"/>
-      <c r="U17" s="118">
+      <c r="B17" s="115"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="115"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="115"/>
+      <c r="N17" s="112"/>
+      <c r="O17" s="114"/>
+      <c r="P17" s="115"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="115"/>
+      <c r="S17" s="115"/>
+      <c r="T17" s="112"/>
+      <c r="U17" s="116">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -21939,7 +21929,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B19" s="78"/>
       <c r="C19" s="78"/>
@@ -21969,44 +21959,44 @@
         <v>114</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J20" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L20" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N20" s="77"/>
-      <c r="O20" s="107" t="s">
-        <v>242</v>
+      <c r="O20" s="105" t="s">
+        <v>241</v>
       </c>
       <c r="P20" s="7"/>
       <c r="Q20" s="77"/>
@@ -22022,44 +22012,44 @@
         <v>115</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J21" s="79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L21" s="79" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M21" s="78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N21" s="79"/>
-      <c r="O21" s="115" t="s">
-        <v>242</v>
+      <c r="O21" s="113" t="s">
+        <v>241</v>
       </c>
       <c r="P21" s="78"/>
       <c r="Q21" s="79"/>
@@ -22075,40 +22065,40 @@
         <v>119</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L22" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N22" s="77"/>
-      <c r="O22" s="107" t="s">
-        <v>242</v>
+      <c r="O22" s="105" t="s">
+        <v>241</v>
       </c>
       <c r="P22" s="7">
         <v>2</v>
@@ -22132,39 +22122,39 @@
         <v>120</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J23" s="82"/>
       <c r="K23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L23" s="82" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N23" s="82"/>
-      <c r="O23" s="108">
+      <c r="O23" s="106">
         <v>0.1</v>
       </c>
       <c r="P23" s="8"/>
@@ -22499,7 +22489,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -22562,7 +22552,7 @@
         <v>119</v>
       </c>
       <c r="B7" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="29">
         <v>0.5</v>
@@ -22573,7 +22563,7 @@
         <v>120</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="29">
         <v>0.5</v>
@@ -22584,7 +22574,7 @@
         <v>119</v>
       </c>
       <c r="B9" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="29">
         <v>0.5</v>
@@ -22595,7 +22585,7 @@
         <v>120</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="29">
         <v>0.5</v>
@@ -22606,7 +22596,7 @@
         <v>119</v>
       </c>
       <c r="B11" s="84" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" s="29">
         <v>0.5</v>
@@ -22617,7 +22607,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="87" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" s="9">
         <v>0.5</v>
@@ -22648,7 +22638,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -22659,7 +22649,7 @@
         <v>233</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -22711,7 +22701,7 @@
         <v>119</v>
       </c>
       <c r="B7" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="29">
         <v>0.99</v>
@@ -22722,7 +22712,7 @@
         <v>120</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="29">
         <v>0.99</v>
@@ -22733,7 +22723,7 @@
         <v>119</v>
       </c>
       <c r="B9" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="29">
         <v>0.99</v>
@@ -22744,7 +22734,7 @@
         <v>120</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" s="29">
         <v>0.99</v>
@@ -22755,7 +22745,7 @@
         <v>119</v>
       </c>
       <c r="B11" s="84" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" s="29">
         <v>0.99</v>
@@ -22766,7 +22756,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="87" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" s="89">
         <v>0.99</v>
@@ -22796,7 +22786,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -22825,7 +22815,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="88" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" s="35">
         <v>1</v>
@@ -22833,7 +22823,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="88" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" s="35">
         <v>1</v>
@@ -22841,7 +22831,7 @@
     </row>
     <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" s="37">
         <v>1</v>
@@ -22871,7 +22861,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -22928,7 +22918,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>46</v>
@@ -22936,7 +22926,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="29">
         <v>0.04</v>
@@ -22944,7 +22934,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="29">
         <v>0.1</v>
@@ -22952,7 +22942,7 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="9">
         <v>0.5</v>
@@ -22988,7 +22978,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>46</v>
@@ -22996,7 +22986,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="29">
         <v>0.25</v>
@@ -23004,7 +22994,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="29">
         <v>0.35</v>
@@ -23012,7 +23002,7 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="9">
         <v>3.3</v>
@@ -23042,7 +23032,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -23086,7 +23076,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -23094,12 +23084,12 @@
         <v>45</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3" s="35">
         <v>110</v>
@@ -23107,7 +23097,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B4" s="41">
         <v>0.03</v>
@@ -23115,24 +23105,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B5" s="35">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B6" s="37">
         <v>150</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -23159,7 +23149,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -23167,12 +23157,12 @@
         <v>45</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3" s="41">
         <v>0.08</v>
@@ -23180,7 +23170,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4" s="37">
         <v>20</v>
@@ -23227,7 +23217,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
@@ -23235,7 +23225,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -23276,10 +23266,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -23354,10 +23344,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -23370,7 +23360,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="49">
         <v>150000</v>
@@ -23378,7 +23368,7 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="50">
         <v>150000</v>
@@ -23418,7 +23408,7 @@
         <v>158</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -23500,19 +23490,19 @@
       <c r="A4" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="131">
-        <v>0</v>
-      </c>
-      <c r="D4" s="125">
+      <c r="C4" s="129">
+        <v>0</v>
+      </c>
+      <c r="D4" s="123">
         <v>68</v>
       </c>
-      <c r="E4" s="125">
+      <c r="E4" s="123">
         <v>70</v>
       </c>
-      <c r="F4" s="126">
+      <c r="F4" s="124">
         <v>72</v>
       </c>
     </row>
@@ -23540,19 +23530,19 @@
       <c r="A6" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="128" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="131">
-        <v>0</v>
-      </c>
-      <c r="D6" s="125">
+      <c r="C6" s="129">
+        <v>0</v>
+      </c>
+      <c r="D6" s="123">
         <v>68</v>
       </c>
-      <c r="E6" s="125">
+      <c r="E6" s="123">
         <v>70</v>
       </c>
-      <c r="F6" s="126">
+      <c r="F6" s="124">
         <v>72</v>
       </c>
     </row>
@@ -23561,7 +23551,7 @@
         <v>119</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C7" s="34">
         <v>0</v>
@@ -23581,19 +23571,19 @@
       <c r="A8" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="130" t="s">
-        <v>255</v>
-      </c>
-      <c r="C8" s="131">
-        <v>0</v>
-      </c>
-      <c r="D8" s="125">
+      <c r="B8" s="128" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="129">
+        <v>0</v>
+      </c>
+      <c r="D8" s="123">
         <v>68</v>
       </c>
-      <c r="E8" s="125">
+      <c r="E8" s="123">
         <v>70</v>
       </c>
-      <c r="F8" s="126">
+      <c r="F8" s="124">
         <v>72</v>
       </c>
       <c r="K8" s="10"/>
@@ -23603,7 +23593,7 @@
         <v>119</v>
       </c>
       <c r="B9" s="76" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" s="34">
         <v>0</v>
@@ -23623,19 +23613,19 @@
       <c r="A10" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="130" t="s">
-        <v>256</v>
-      </c>
-      <c r="C10" s="131">
-        <v>0</v>
-      </c>
-      <c r="D10" s="125">
+      <c r="B10" s="128" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="129">
+        <v>0</v>
+      </c>
+      <c r="D10" s="123">
         <v>68</v>
       </c>
-      <c r="E10" s="125">
+      <c r="E10" s="123">
         <v>70</v>
       </c>
-      <c r="F10" s="126">
+      <c r="F10" s="124">
         <v>72</v>
       </c>
       <c r="K10" s="10"/>
@@ -23645,7 +23635,7 @@
         <v>119</v>
       </c>
       <c r="B11" s="76" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" s="34">
         <v>0</v>
@@ -23666,7 +23656,7 @@
         <v>120</v>
       </c>
       <c r="B12" s="85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12" s="36">
         <v>0</v>
@@ -23800,7 +23790,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="34">
         <v>0</v>
@@ -23817,7 +23807,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B5" s="36">
         <v>0</v>
@@ -23862,14 +23852,14 @@
         <v>45</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="B3" s="132">
+        <v>288</v>
+      </c>
+      <c r="B3" s="130">
         <v>0.2</v>
       </c>
     </row>
@@ -23919,16 +23909,16 @@
       <c r="A3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="131" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="134">
-        <v>0</v>
-      </c>
-      <c r="D3" s="134">
+      <c r="C3" s="132">
+        <v>0</v>
+      </c>
+      <c r="D3" s="132">
         <v>1</v>
       </c>
-      <c r="E3" s="127">
+      <c r="E3" s="125">
         <v>2</v>
       </c>
     </row>
@@ -23936,16 +23926,16 @@
       <c r="A4" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="131" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="134">
-        <v>0</v>
-      </c>
-      <c r="D4" s="134">
+      <c r="C4" s="132">
+        <v>0</v>
+      </c>
+      <c r="D4" s="132">
         <v>1</v>
       </c>
-      <c r="E4" s="127">
+      <c r="E4" s="125">
         <v>2</v>
       </c>
     </row>
@@ -23953,16 +23943,16 @@
       <c r="A5" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="131" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="134">
-        <v>0</v>
-      </c>
-      <c r="D5" s="134">
+      <c r="C5" s="132">
+        <v>0</v>
+      </c>
+      <c r="D5" s="132">
         <v>1</v>
       </c>
-      <c r="E5" s="127">
+      <c r="E5" s="125">
         <v>2</v>
       </c>
     </row>
@@ -23970,16 +23960,16 @@
       <c r="A6" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="133" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="128">
-        <v>0</v>
-      </c>
-      <c r="D6" s="128">
+      <c r="C6" s="126">
+        <v>0</v>
+      </c>
+      <c r="D6" s="126">
         <v>1</v>
       </c>
-      <c r="E6" s="129">
+      <c r="E6" s="127">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tabs to support data required for seismicity risk calculations
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E30C186-FA0E-4A41-B4B2-36644D841BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D2CBBD-4812-4EAE-99B6-C4299250DBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -110,6 +110,11 @@
     <sheet name="StorageExpansionLeadTime" sheetId="130" r:id="rId95"/>
     <sheet name="PipelineExpansionLeadTime_Dist" sheetId="131" r:id="rId96"/>
     <sheet name="PipelineExpansionLeadTime_Capac" sheetId="132" r:id="rId97"/>
+    <sheet name="SWDProxAbandWell" sheetId="137" r:id="rId98"/>
+    <sheet name="SWDProxInacWell" sheetId="139" r:id="rId99"/>
+    <sheet name="SWDProxEQ" sheetId="140" r:id="rId100"/>
+    <sheet name="SWDProxFault" sheetId="141" r:id="rId101"/>
+    <sheet name="SWDProxHpOrLpWell" sheetId="142" r:id="rId102"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
@@ -136,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="296">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1009,6 +1014,21 @@
   </si>
   <si>
     <t>Treatment Sites to Disposal Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to abandoned well (miles)</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to inactive formerly producing well (completed prior to 2000) (miles)</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to earthquakes &gt;= 3.0 (miles)</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to fault (miles)</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to high pressure (&gt; 0.7 psi) or low pressure (&lt; 0.5 psi) injection well (miles)</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1678,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1974,6 +1994,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3015,6 +3063,162 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CD8121-8E85-4F4C-B060-AFA9C3041DD8}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="134"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="142" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="140" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="138">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="139">
+        <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81F533B-E9FD-4761-8F4E-5B669BFE9F9E}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="134"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="142" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="140" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="138">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="139">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A75715-B1AD-4143-9F27-64608123485A}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="134"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="142" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="140" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="138">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="139">
+        <v>5.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C820352-28DB-4692-BCE8-9A9846CC4956}">
   <sheetPr>
@@ -20407,7 +20611,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23976,4 +24180,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E511B3-01EE-48B4-88CB-240156F02C0C}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="134" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="134" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="134" customWidth="1"/>
+    <col min="4" max="5" width="25.140625" style="134" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="134" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="134"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="142" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="140" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="138">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="139">
+        <v>1.3</v>
+      </c>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D275CFA9-875E-41E8-B7DD-F33879DC506B}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="134" customWidth="1"/>
+    <col min="2" max="3" width="9.5703125" style="134" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="134"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="142" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="140" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="138">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="139">
+        <v>2.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add additional tabs required for seismicity risk analysis
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_toy_case_study.xlsx
+++ b/pareto/case_studies/strategic_toy_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D2CBBD-4812-4EAE-99B6-C4299250DBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176D1AC7-559C-488F-B69C-70365E13200B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -110,11 +110,14 @@
     <sheet name="StorageExpansionLeadTime" sheetId="130" r:id="rId95"/>
     <sheet name="PipelineExpansionLeadTime_Dist" sheetId="131" r:id="rId96"/>
     <sheet name="PipelineExpansionLeadTime_Capac" sheetId="132" r:id="rId97"/>
-    <sheet name="SWDProxAbandWell" sheetId="137" r:id="rId98"/>
-    <sheet name="SWDProxInacWell" sheetId="139" r:id="rId99"/>
-    <sheet name="SWDProxEQ" sheetId="140" r:id="rId100"/>
-    <sheet name="SWDProxFault" sheetId="141" r:id="rId101"/>
-    <sheet name="SWDProxHpOrLpWell" sheetId="142" r:id="rId102"/>
+    <sheet name="SWDDeep" sheetId="144" r:id="rId98"/>
+    <sheet name="SWDAveragePressure" sheetId="145" r:id="rId99"/>
+    <sheet name="SWDProxOrphanWell" sheetId="137" r:id="rId100"/>
+    <sheet name="SWDProxInactiveWell" sheetId="139" r:id="rId101"/>
+    <sheet name="SWDProxEQ" sheetId="140" r:id="rId102"/>
+    <sheet name="SWDProxFault" sheetId="141" r:id="rId103"/>
+    <sheet name="SWDProxHpOrLpWell" sheetId="142" r:id="rId104"/>
+    <sheet name="SWDRiskFactors" sheetId="143" r:id="rId105"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
@@ -141,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="312">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1016,19 +1019,67 @@
     <t>Treatment Sites to Disposal Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
   <si>
-    <t>Table of SWD proximity to abandoned well (miles)</t>
-  </si>
-  <si>
-    <t>Table of SWD proximity to inactive formerly producing well (completed prior to 2000) (miles)</t>
-  </si>
-  <si>
-    <t>Table of SWD proximity to earthquakes &gt;= 3.0 (miles)</t>
-  </si>
-  <si>
-    <t>Table of SWD proximity to fault (miles)</t>
-  </si>
-  <si>
-    <t>Table of SWD proximity to high pressure (&gt; 0.7 psi) or low pressure (&lt; 0.5 psi) injection well (miles)</t>
+    <t>orphan_well_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>orphan_well_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>inactive_well_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>inactive_well_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>EQ_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>EQ_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>Average pressure/depth in vicinity of well [psi/ft]</t>
+  </si>
+  <si>
+    <t>SWDs - shallow (0) or deep (1)</t>
+  </si>
+  <si>
+    <t>fault_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>fault_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_LP_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_LP_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_threshold</t>
+  </si>
+  <si>
+    <t>LP_threshold</t>
+  </si>
+  <si>
+    <t>psi/ft</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to orphan well [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to inactive/temporarily abandoned formerly producing well (completed prior to 2000) [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to earthquakes &gt;= 3.0 magnitude [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to fault [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to high pressure or low pressure injection well [miles]</t>
+  </si>
+  <si>
+    <t>SWD risk factors</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1729,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1995,33 +2046,36 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3064,6 +3118,133 @@
 </file>
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E511B3-01EE-48B4-88CB-240156F02C0C}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0.15</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D275CFA9-875E-41E8-B7DD-F33879DC506B}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="29">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CD8121-8E85-4F4C-B060-AFA9C3041DD8}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
@@ -3081,33 +3262,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
-        <v>293</v>
-      </c>
-      <c r="B1" s="134"/>
+      <c r="A1" s="1" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="136" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="138">
-        <v>3.4</v>
+      <c r="B3" s="29">
+        <v>3.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="139">
-        <v>3.5</v>
+      <c r="B4" s="9">
+        <v>3.88</v>
       </c>
     </row>
   </sheetData>
@@ -3115,7 +3295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81F533B-E9FD-4761-8F4E-5B669BFE9F9E}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
@@ -3133,33 +3313,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
-        <v>294</v>
-      </c>
-      <c r="B1" s="134"/>
+      <c r="A1" s="1" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="136" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="138">
-        <v>4.5</v>
+      <c r="B3" s="29">
+        <v>4.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="139">
-        <v>4.5999999999999996</v>
+      <c r="B4" s="9">
+        <v>7.23</v>
       </c>
     </row>
   </sheetData>
@@ -3167,7 +3346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A75715-B1AD-4143-9F27-64608123485A}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
@@ -3185,36 +3364,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="29">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81219482-3A41-42E9-B4D8-D927BFC48D38}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" style="138" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="138"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="137" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="139" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="140" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="141" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="142">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="141" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" s="142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="141" t="s">
+        <v>293</v>
+      </c>
+      <c r="B5" s="142">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="141" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" s="142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="141" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="134"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" s="143" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="138">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="139">
-        <v>5.7</v>
+      <c r="B7" s="142">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="141" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" s="142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="141" t="s">
+        <v>299</v>
+      </c>
+      <c r="B9" s="142">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="141" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" s="142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="141" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" s="142">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="141" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" s="142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="141" t="s">
+        <v>303</v>
+      </c>
+      <c r="B13" s="142">
+        <v>0.7</v>
+      </c>
+      <c r="C13" s="138" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="143" t="s">
+        <v>304</v>
+      </c>
+      <c r="B14" s="144">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="138" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20611,7 +20927,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23342,7 +23658,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24183,11 +24499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E511B3-01EE-48B4-88CB-240156F02C0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D360A16-D4D1-450C-881A-205060A78B8B}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -24195,58 +24511,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="134" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="134" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="134" customWidth="1"/>
-    <col min="4" max="5" width="25.140625" style="134" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="134" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="134"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="136" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="138">
-        <v>1.2</v>
-      </c>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141" t="s">
+      <c r="B3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="139">
-        <v>1.3</v>
-      </c>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
-      <c r="F4" s="137"/>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24254,11 +24550,11 @@
 </file>
 
 <file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D275CFA9-875E-41E8-B7DD-F33879DC506B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A6B482-DAE2-4301-B427-8F96394EDBA4}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -24266,42 +24562,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="134" customWidth="1"/>
-    <col min="2" max="3" width="9.5703125" style="134" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="134"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="142" t="s">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="136" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="140" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="138">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141" t="s">
+      <c r="B3" s="29">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="139">
-        <v>2.4</v>
+      <c r="B4" s="9">
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>